<commit_message>
- Added ColTypes and Guess Functionality to readExcel function
Signed-off-by: LeandroC89 <leandroadao3@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/krangl/data/ExcelReadExample.xlsx
+++ b/src/test/resources/krangl/data/ExcelReadExample.xlsx
@@ -5,23 +5,33 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LCouto\IdeaProjects\kchecked\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LCouto\IdeaProjects\krangl\src\test\resources\krangl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A66FDC5-4C8D-4A75-A1AC-B4F7C4C49B21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226F6E08-875A-4E70-94FD-9DD232600BAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5115" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstSheet" sheetId="1" r:id="rId1"/>
     <sheet name="SecondSheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="389">
   <si>
     <t>Name</t>
   </si>
@@ -1182,6 +1192,12 @@
   </si>
   <si>
     <t>30/08/1978</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Registered</t>
   </si>
 </sst>
 </file>
@@ -1522,7 +1538,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1534,7 +1550,7 @@
     <col min="4" max="4" width="35.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1547,8 +1563,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>387</v>
+      </c>
+      <c r="F1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1561,8 +1583,14 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1575,8 +1603,14 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>17</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1589,8 +1623,14 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>14</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1603,8 +1643,14 @@
       <c r="D5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>10</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1617,8 +1663,14 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1631,8 +1683,14 @@
       <c r="D7" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>18</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1645,8 +1703,14 @@
       <c r="D8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1659,8 +1723,14 @@
       <c r="D9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>16</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1673,8 +1743,14 @@
       <c r="D10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1687,8 +1763,14 @@
       <c r="D11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1701,8 +1783,14 @@
       <c r="D12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1715,8 +1803,14 @@
       <c r="D13" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1729,8 +1823,14 @@
       <c r="D14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1743,8 +1843,14 @@
       <c r="D15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1757,8 +1863,14 @@
       <c r="D16" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>14</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1771,8 +1883,14 @@
       <c r="D17" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>8</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1785,8 +1903,14 @@
       <c r="D18" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>13</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -1799,8 +1923,14 @@
       <c r="D19" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>7</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -1813,8 +1943,14 @@
       <c r="D20" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1827,8 +1963,14 @@
       <c r="D21" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>8</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1841,8 +1983,14 @@
       <c r="D22" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>16</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -1855,8 +2003,14 @@
       <c r="D23" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -1869,8 +2023,14 @@
       <c r="D24" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>13</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -1883,8 +2043,14 @@
       <c r="D25" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -1897,8 +2063,14 @@
       <c r="D26" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>7</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -1911,8 +2083,14 @@
       <c r="D27" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>12</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -1925,8 +2103,14 @@
       <c r="D28" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -1939,8 +2123,14 @@
       <c r="D29" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -1953,8 +2143,14 @@
       <c r="D30" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>120</v>
       </c>
@@ -1967,8 +2163,14 @@
       <c r="D31" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>14</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>124</v>
       </c>
@@ -1981,8 +2183,14 @@
       <c r="D32" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>10</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>128</v>
       </c>
@@ -1995,8 +2203,14 @@
       <c r="D33" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>132</v>
       </c>
@@ -2009,8 +2223,14 @@
       <c r="D34" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>11</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>136</v>
       </c>
@@ -2023,8 +2243,14 @@
       <c r="D35" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>139</v>
       </c>
@@ -2037,8 +2263,14 @@
       <c r="D36" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>13</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>143</v>
       </c>
@@ -2051,8 +2283,14 @@
       <c r="D37" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>6</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -2065,8 +2303,14 @@
       <c r="D38" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>5</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -2079,8 +2323,14 @@
       <c r="D39" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>17</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>155</v>
       </c>
@@ -2093,8 +2343,14 @@
       <c r="D40" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>158</v>
       </c>
@@ -2107,8 +2363,14 @@
       <c r="D41" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>16</v>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>136</v>
       </c>
@@ -2121,8 +2383,14 @@
       <c r="D42" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>165</v>
       </c>
@@ -2135,8 +2403,14 @@
       <c r="D43" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>169</v>
       </c>
@@ -2149,8 +2423,14 @@
       <c r="D44" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>173</v>
       </c>
@@ -2163,8 +2443,14 @@
       <c r="D45" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>177</v>
       </c>
@@ -2177,8 +2463,14 @@
       <c r="D46" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>6</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>181</v>
       </c>
@@ -2191,8 +2483,14 @@
       <c r="D47" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>20</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>184</v>
       </c>
@@ -2205,8 +2503,14 @@
       <c r="D48" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>188</v>
       </c>
@@ -2219,8 +2523,14 @@
       <c r="D49" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>19</v>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>192</v>
       </c>
@@ -2233,8 +2543,14 @@
       <c r="D50" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>196</v>
       </c>
@@ -2247,8 +2563,14 @@
       <c r="D51" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>15</v>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>200</v>
       </c>
@@ -2261,8 +2583,14 @@
       <c r="D52" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>20</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>204</v>
       </c>
@@ -2275,8 +2603,14 @@
       <c r="D53" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>10</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>208</v>
       </c>
@@ -2289,8 +2623,14 @@
       <c r="D54" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>17</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>212</v>
       </c>
@@ -2303,8 +2643,14 @@
       <c r="D55" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>216</v>
       </c>
@@ -2317,8 +2663,14 @@
       <c r="D56" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>11</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>220</v>
       </c>
@@ -2331,8 +2683,14 @@
       <c r="D57" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>13</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>224</v>
       </c>
@@ -2345,8 +2703,14 @@
       <c r="D58" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>227</v>
       </c>
@@ -2359,8 +2723,14 @@
       <c r="D59" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>9</v>
+      </c>
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>231</v>
       </c>
@@ -2373,8 +2743,14 @@
       <c r="D60" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>235</v>
       </c>
@@ -2387,8 +2763,14 @@
       <c r="D61" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>3</v>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>239</v>
       </c>
@@ -2401,8 +2783,14 @@
       <c r="D62" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>18</v>
+      </c>
+      <c r="F62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>242</v>
       </c>
@@ -2415,8 +2803,14 @@
       <c r="D63" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>8</v>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>246</v>
       </c>
@@ -2429,8 +2823,14 @@
       <c r="D64" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>7</v>
+      </c>
+      <c r="F64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>250</v>
       </c>
@@ -2443,8 +2843,14 @@
       <c r="D65" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>254</v>
       </c>
@@ -2457,8 +2863,14 @@
       <c r="D66" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>7</v>
+      </c>
+      <c r="F66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>257</v>
       </c>
@@ -2471,8 +2883,14 @@
       <c r="D67" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>17</v>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>261</v>
       </c>
@@ -2485,8 +2903,14 @@
       <c r="D68" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>6</v>
+      </c>
+      <c r="F68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>265</v>
       </c>
@@ -2499,8 +2923,14 @@
       <c r="D69" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>20</v>
+      </c>
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>268</v>
       </c>
@@ -2513,8 +2943,14 @@
       <c r="D70" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>11</v>
+      </c>
+      <c r="F70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>272</v>
       </c>
@@ -2527,8 +2963,14 @@
       <c r="D71" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>1</v>
+      </c>
+      <c r="F71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -2541,8 +2983,14 @@
       <c r="D72" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>13</v>
+      </c>
+      <c r="F72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>278</v>
       </c>
@@ -2555,8 +3003,14 @@
       <c r="D73" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>16</v>
+      </c>
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>282</v>
       </c>
@@ -2569,8 +3023,14 @@
       <c r="D74" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>10</v>
+      </c>
+      <c r="F74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>286</v>
       </c>
@@ -2583,8 +3043,14 @@
       <c r="D75" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>13</v>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>289</v>
       </c>
@@ -2597,8 +3063,14 @@
       <c r="D76" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>8</v>
+      </c>
+      <c r="F76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>293</v>
       </c>
@@ -2611,8 +3083,14 @@
       <c r="D77" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>7</v>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>297</v>
       </c>
@@ -2625,8 +3103,14 @@
       <c r="D78" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>4</v>
+      </c>
+      <c r="F78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>300</v>
       </c>
@@ -2639,8 +3123,14 @@
       <c r="D79" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>13</v>
+      </c>
+      <c r="F79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>304</v>
       </c>
@@ -2653,8 +3143,14 @@
       <c r="D80" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>17</v>
+      </c>
+      <c r="F80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>308</v>
       </c>
@@ -2667,8 +3163,14 @@
       <c r="D81" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>12</v>
+      </c>
+      <c r="F81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>312</v>
       </c>
@@ -2681,8 +3183,14 @@
       <c r="D82" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>15</v>
+      </c>
+      <c r="F82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>315</v>
       </c>
@@ -2695,8 +3203,14 @@
       <c r="D83" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>15</v>
+      </c>
+      <c r="F83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>319</v>
       </c>
@@ -2709,8 +3223,14 @@
       <c r="D84" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>19</v>
+      </c>
+      <c r="F84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>323</v>
       </c>
@@ -2723,8 +3243,14 @@
       <c r="D85" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>12</v>
+      </c>
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>327</v>
       </c>
@@ -2737,8 +3263,14 @@
       <c r="D86" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>14</v>
+      </c>
+      <c r="F86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>331</v>
       </c>
@@ -2751,8 +3283,14 @@
       <c r="D87" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>3</v>
+      </c>
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>335</v>
       </c>
@@ -2765,8 +3303,14 @@
       <c r="D88" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>2</v>
+      </c>
+      <c r="F88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>339</v>
       </c>
@@ -2779,8 +3323,14 @@
       <c r="D89" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>2</v>
+      </c>
+      <c r="F89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>343</v>
       </c>
@@ -2793,8 +3343,14 @@
       <c r="D90" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>16</v>
+      </c>
+      <c r="F90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>346</v>
       </c>
@@ -2807,8 +3363,14 @@
       <c r="D91" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>19</v>
+      </c>
+      <c r="F91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>349</v>
       </c>
@@ -2821,8 +3383,14 @@
       <c r="D92" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>9</v>
+      </c>
+      <c r="F92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>353</v>
       </c>
@@ -2835,8 +3403,14 @@
       <c r="D93" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>10</v>
+      </c>
+      <c r="F93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>356</v>
       </c>
@@ -2849,8 +3423,14 @@
       <c r="D94" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>360</v>
       </c>
@@ -2863,8 +3443,14 @@
       <c r="D95" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>1</v>
+      </c>
+      <c r="F95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>364</v>
       </c>
@@ -2877,8 +3463,14 @@
       <c r="D96" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>2</v>
+      </c>
+      <c r="F96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>368</v>
       </c>
@@ -2891,8 +3483,14 @@
       <c r="D97" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>19</v>
+      </c>
+      <c r="F97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>372</v>
       </c>
@@ -2905,8 +3503,14 @@
       <c r="D98" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>16</v>
+      </c>
+      <c r="F98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>376</v>
       </c>
@@ -2919,8 +3523,14 @@
       <c r="D99" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>1</v>
+      </c>
+      <c r="F99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>380</v>
       </c>
@@ -2933,8 +3543,14 @@
       <c r="D100" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>8</v>
+      </c>
+      <c r="F100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>384</v>
       </c>
@@ -2946,6 +3562,12 @@
       </c>
       <c r="D101" t="s">
         <v>15</v>
+      </c>
+      <c r="E101">
+        <v>13</v>
+      </c>
+      <c r="F101" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2956,15 +3578,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D48153-1644-422E-BF6C-88BBA322D82D}">
-  <dimension ref="A3:D103"/>
+  <dimension ref="A3:F103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2977,8 +3597,14 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>387</v>
+      </c>
+      <c r="F3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2991,8 +3617,14 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3005,8 +3637,14 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>17</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -3019,8 +3657,14 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>14</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -3033,8 +3677,14 @@
       <c r="D7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -3047,8 +3697,14 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -3061,8 +3717,14 @@
       <c r="D9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>18</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -3075,8 +3737,14 @@
       <c r="D10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -3089,8 +3757,14 @@
       <c r="D11" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>16</v>
+      </c>
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -3103,8 +3777,14 @@
       <c r="D12" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -3117,8 +3797,14 @@
       <c r="D13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>7</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -3131,8 +3817,14 @@
       <c r="D14" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -3145,8 +3837,14 @@
       <c r="D15" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -3159,8 +3857,14 @@
       <c r="D16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -3173,8 +3877,14 @@
       <c r="D17" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -3187,8 +3897,14 @@
       <c r="D18" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>14</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>64</v>
       </c>
@@ -3201,8 +3917,14 @@
       <c r="D19" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>68</v>
       </c>
@@ -3215,8 +3937,14 @@
       <c r="D20" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>13</v>
+      </c>
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -3229,8 +3957,14 @@
       <c r="D21" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>7</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -3243,8 +3977,14 @@
       <c r="D22" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>80</v>
       </c>
@@ -3257,8 +3997,14 @@
       <c r="D23" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>84</v>
       </c>
@@ -3271,8 +4017,14 @@
       <c r="D24" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>16</v>
+      </c>
+      <c r="F24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>88</v>
       </c>
@@ -3285,8 +4037,14 @@
       <c r="D25" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>92</v>
       </c>
@@ -3299,8 +4057,14 @@
       <c r="D26" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>13</v>
+      </c>
+      <c r="F26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>96</v>
       </c>
@@ -3313,8 +4077,14 @@
       <c r="D27" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>100</v>
       </c>
@@ -3327,8 +4097,14 @@
       <c r="D28" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -3341,8 +4117,14 @@
       <c r="D29" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>12</v>
+      </c>
+      <c r="F29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>108</v>
       </c>
@@ -3355,8 +4137,14 @@
       <c r="D30" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>112</v>
       </c>
@@ -3369,8 +4157,14 @@
       <c r="D31" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>116</v>
       </c>
@@ -3383,8 +4177,14 @@
       <c r="D32" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>7</v>
+      </c>
+      <c r="F32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -3397,8 +4197,14 @@
       <c r="D33" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>14</v>
+      </c>
+      <c r="F33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>124</v>
       </c>
@@ -3411,8 +4217,14 @@
       <c r="D34" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>10</v>
+      </c>
+      <c r="F34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>128</v>
       </c>
@@ -3425,8 +4237,14 @@
       <c r="D35" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>4</v>
+      </c>
+      <c r="F35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>132</v>
       </c>
@@ -3439,8 +4257,14 @@
       <c r="D36" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>11</v>
+      </c>
+      <c r="F36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>136</v>
       </c>
@@ -3453,8 +4277,14 @@
       <c r="D37" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>139</v>
       </c>
@@ -3467,8 +4297,14 @@
       <c r="D38" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>13</v>
+      </c>
+      <c r="F38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>143</v>
       </c>
@@ -3481,8 +4317,14 @@
       <c r="D39" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>6</v>
+      </c>
+      <c r="F39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -3495,8 +4337,14 @@
       <c r="D40" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>5</v>
+      </c>
+      <c r="F40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>151</v>
       </c>
@@ -3509,8 +4357,14 @@
       <c r="D41" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>17</v>
+      </c>
+      <c r="F41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>155</v>
       </c>
@@ -3523,8 +4377,14 @@
       <c r="D42" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>158</v>
       </c>
@@ -3537,8 +4397,14 @@
       <c r="D43" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>16</v>
+      </c>
+      <c r="F43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>136</v>
       </c>
@@ -3551,8 +4417,14 @@
       <c r="D44" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>165</v>
       </c>
@@ -3565,8 +4437,14 @@
       <c r="D45" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>169</v>
       </c>
@@ -3579,8 +4457,14 @@
       <c r="D46" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>173</v>
       </c>
@@ -3593,8 +4477,14 @@
       <c r="D47" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>177</v>
       </c>
@@ -3607,8 +4497,14 @@
       <c r="D48" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>6</v>
+      </c>
+      <c r="F48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>181</v>
       </c>
@@ -3621,8 +4517,14 @@
       <c r="D49" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>20</v>
+      </c>
+      <c r="F49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>184</v>
       </c>
@@ -3635,8 +4537,14 @@
       <c r="D50" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>188</v>
       </c>
@@ -3649,8 +4557,14 @@
       <c r="D51" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>19</v>
+      </c>
+      <c r="F51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>192</v>
       </c>
@@ -3663,8 +4577,14 @@
       <c r="D52" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>196</v>
       </c>
@@ -3677,8 +4597,14 @@
       <c r="D53" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>15</v>
+      </c>
+      <c r="F53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>200</v>
       </c>
@@ -3691,8 +4617,14 @@
       <c r="D54" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>20</v>
+      </c>
+      <c r="F54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>204</v>
       </c>
@@ -3705,8 +4637,14 @@
       <c r="D55" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>10</v>
+      </c>
+      <c r="F55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>208</v>
       </c>
@@ -3719,8 +4657,14 @@
       <c r="D56" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>17</v>
+      </c>
+      <c r="F56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>212</v>
       </c>
@@ -3733,8 +4677,14 @@
       <c r="D57" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>216</v>
       </c>
@@ -3747,8 +4697,14 @@
       <c r="D58" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>11</v>
+      </c>
+      <c r="F58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>220</v>
       </c>
@@ -3761,8 +4717,14 @@
       <c r="D59" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>13</v>
+      </c>
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>224</v>
       </c>
@@ -3775,8 +4737,14 @@
       <c r="D60" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="F60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>227</v>
       </c>
@@ -3789,8 +4757,14 @@
       <c r="D61" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>9</v>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>231</v>
       </c>
@@ -3803,8 +4777,14 @@
       <c r="D62" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>235</v>
       </c>
@@ -3817,8 +4797,14 @@
       <c r="D63" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>3</v>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>239</v>
       </c>
@@ -3831,8 +4817,14 @@
       <c r="D64" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>18</v>
+      </c>
+      <c r="F64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>242</v>
       </c>
@@ -3845,8 +4837,14 @@
       <c r="D65" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>8</v>
+      </c>
+      <c r="F65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>246</v>
       </c>
@@ -3859,8 +4857,14 @@
       <c r="D66" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>7</v>
+      </c>
+      <c r="F66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>250</v>
       </c>
@@ -3873,8 +4877,14 @@
       <c r="D67" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>254</v>
       </c>
@@ -3887,8 +4897,14 @@
       <c r="D68" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>7</v>
+      </c>
+      <c r="F68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>257</v>
       </c>
@@ -3901,8 +4917,14 @@
       <c r="D69" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>17</v>
+      </c>
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>261</v>
       </c>
@@ -3915,8 +4937,14 @@
       <c r="D70" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>6</v>
+      </c>
+      <c r="F70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>265</v>
       </c>
@@ -3929,8 +4957,14 @@
       <c r="D71" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>20</v>
+      </c>
+      <c r="F71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>268</v>
       </c>
@@ -3943,8 +4977,14 @@
       <c r="D72" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>11</v>
+      </c>
+      <c r="F72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>272</v>
       </c>
@@ -3957,8 +4997,14 @@
       <c r="D73" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>40</v>
       </c>
@@ -3971,8 +5017,14 @@
       <c r="D74" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>13</v>
+      </c>
+      <c r="F74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>278</v>
       </c>
@@ -3985,8 +5037,14 @@
       <c r="D75" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>16</v>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>282</v>
       </c>
@@ -3999,8 +5057,14 @@
       <c r="D76" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>10</v>
+      </c>
+      <c r="F76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>286</v>
       </c>
@@ -4013,8 +5077,14 @@
       <c r="D77" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>13</v>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>289</v>
       </c>
@@ -4027,8 +5097,14 @@
       <c r="D78" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>8</v>
+      </c>
+      <c r="F78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>293</v>
       </c>
@@ -4041,8 +5117,14 @@
       <c r="D79" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>7</v>
+      </c>
+      <c r="F79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>297</v>
       </c>
@@ -4055,8 +5137,14 @@
       <c r="D80" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>4</v>
+      </c>
+      <c r="F80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>300</v>
       </c>
@@ -4069,8 +5157,14 @@
       <c r="D81" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>13</v>
+      </c>
+      <c r="F81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>304</v>
       </c>
@@ -4083,8 +5177,14 @@
       <c r="D82" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>17</v>
+      </c>
+      <c r="F82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>308</v>
       </c>
@@ -4097,8 +5197,14 @@
       <c r="D83" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>12</v>
+      </c>
+      <c r="F83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>312</v>
       </c>
@@ -4111,8 +5217,14 @@
       <c r="D84" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>15</v>
+      </c>
+      <c r="F84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>315</v>
       </c>
@@ -4125,8 +5237,14 @@
       <c r="D85" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>15</v>
+      </c>
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>319</v>
       </c>
@@ -4139,8 +5257,14 @@
       <c r="D86" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>19</v>
+      </c>
+      <c r="F86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>323</v>
       </c>
@@ -4153,8 +5277,14 @@
       <c r="D87" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>12</v>
+      </c>
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>327</v>
       </c>
@@ -4167,8 +5297,14 @@
       <c r="D88" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>14</v>
+      </c>
+      <c r="F88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>331</v>
       </c>
@@ -4181,8 +5317,14 @@
       <c r="D89" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>3</v>
+      </c>
+      <c r="F89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>335</v>
       </c>
@@ -4195,8 +5337,14 @@
       <c r="D90" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>2</v>
+      </c>
+      <c r="F90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>339</v>
       </c>
@@ -4209,8 +5357,14 @@
       <c r="D91" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>2</v>
+      </c>
+      <c r="F91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>343</v>
       </c>
@@ -4223,8 +5377,14 @@
       <c r="D92" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>16</v>
+      </c>
+      <c r="F92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>346</v>
       </c>
@@ -4237,8 +5397,14 @@
       <c r="D93" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>19</v>
+      </c>
+      <c r="F93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>349</v>
       </c>
@@ -4251,8 +5417,14 @@
       <c r="D94" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>9</v>
+      </c>
+      <c r="F94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>353</v>
       </c>
@@ -4265,8 +5437,14 @@
       <c r="D95" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>10</v>
+      </c>
+      <c r="F95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>356</v>
       </c>
@@ -4279,8 +5457,14 @@
       <c r="D96" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="F96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>360</v>
       </c>
@@ -4293,8 +5477,14 @@
       <c r="D97" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>1</v>
+      </c>
+      <c r="F97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>364</v>
       </c>
@@ -4307,8 +5497,14 @@
       <c r="D98" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>2</v>
+      </c>
+      <c r="F98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>368</v>
       </c>
@@ -4321,8 +5517,14 @@
       <c r="D99" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>19</v>
+      </c>
+      <c r="F99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>372</v>
       </c>
@@ -4335,8 +5537,14 @@
       <c r="D100" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>16</v>
+      </c>
+      <c r="F100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>376</v>
       </c>
@@ -4349,8 +5557,14 @@
       <c r="D101" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>1</v>
+      </c>
+      <c r="F101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>380</v>
       </c>
@@ -4363,8 +5577,14 @@
       <c r="D102" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102">
+        <v>8</v>
+      </c>
+      <c r="F102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>384</v>
       </c>
@@ -4376,6 +5596,12 @@
       </c>
       <c r="D103" t="s">
         <v>15</v>
+      </c>
+      <c r="E103">
+        <v>13</v>
+      </c>
+      <c r="F103" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Added trim_ws functionality from read_excel
Signed-off-by: LeandroC89 <leandroadao3@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/krangl/data/ExcelReadExample.xlsx
+++ b/src/test/resources/krangl/data/ExcelReadExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LCouto\IdeaProjects\krangl\src\test\resources\krangl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{226F6E08-875A-4E70-94FD-9DD232600BAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E90D4C1-E0F3-49AE-8E80-58884565C9AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5115" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstSheet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="390">
   <si>
     <t>Name</t>
   </si>
@@ -405,799 +405,802 @@
     <t>India</t>
   </si>
   <si>
+    <t>29/11/1986</t>
+  </si>
+  <si>
+    <t>Holy See (Vatican City State)</t>
+  </si>
+  <si>
+    <t>Quamar</t>
+  </si>
+  <si>
+    <t>gravida.non@Aliquamornare.edu</t>
+  </si>
+  <si>
+    <t>27/07/1994</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Lacota</t>
+  </si>
+  <si>
+    <t>facilisis@Proinnon.com</t>
+  </si>
+  <si>
+    <t>29/05/1984</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Sylvester</t>
+  </si>
+  <si>
+    <t>sagittis.lobortis.mauris@loremsitamet.org</t>
+  </si>
+  <si>
+    <t>02/03/1979</t>
+  </si>
+  <si>
+    <t>Sloane</t>
+  </si>
+  <si>
+    <t>vulputate@senectus.com</t>
+  </si>
+  <si>
+    <t>06/05/1998</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Arthur</t>
+  </si>
+  <si>
+    <t>cursus.purus@risusaultricies.edu</t>
+  </si>
+  <si>
+    <t>14/10/1997</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Hakeem</t>
+  </si>
+  <si>
+    <t>nec.luctus@hendreritidante.ca</t>
+  </si>
+  <si>
+    <t>10/02/1972</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Fritz</t>
+  </si>
+  <si>
+    <t>molestie.Sed.id@adipiscingelitCurabitur.org</t>
+  </si>
+  <si>
+    <t>21/05/2002</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Callum</t>
+  </si>
+  <si>
+    <t>fringilla.cursus.purus@ultrices.co.uk</t>
+  </si>
+  <si>
+    <t>08/07/1991</t>
+  </si>
+  <si>
+    <t>Rinah</t>
+  </si>
+  <si>
+    <t>morbi@lacuspedesagittis.edu</t>
+  </si>
+  <si>
+    <t>10/03/1998</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>interdum@infelis.net</t>
+  </si>
+  <si>
+    <t>16/09/1996</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Demetria</t>
+  </si>
+  <si>
+    <t>Donec@pharetraQuisqueac.org</t>
+  </si>
+  <si>
+    <t>08/07/1984</t>
+  </si>
+  <si>
+    <t>Western Sahara</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>sociosqu.ad@lectusconvallisest.ca</t>
+  </si>
+  <si>
+    <t>27/11/1987</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Cole</t>
+  </si>
+  <si>
+    <t>amet.luctus.vulputate@non.co.uk</t>
+  </si>
+  <si>
+    <t>22/04/1989</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
+  </si>
+  <si>
+    <t>Oscar</t>
+  </si>
+  <si>
+    <t>mattis.ornare.lectus@IncondimentumDonec.net</t>
+  </si>
+  <si>
+    <t>17/01/1980</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Kaitlin</t>
+  </si>
+  <si>
+    <t>luctus@metusurnaconvallis.ca</t>
+  </si>
+  <si>
+    <t>10/06/1976</t>
+  </si>
+  <si>
+    <t>Raymond</t>
+  </si>
+  <si>
+    <t>Quisque@Donecdignissimmagna.ca</t>
+  </si>
+  <si>
+    <t>26/10/2001</t>
+  </si>
+  <si>
+    <t>Saint Martin</t>
+  </si>
+  <si>
+    <t>Allegra</t>
+  </si>
+  <si>
+    <t>blandit.Nam.nulla@aliquetmetus.ca</t>
+  </si>
+  <si>
+    <t>11/11/1994</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Elliott</t>
+  </si>
+  <si>
+    <t>orci@feugiat.com</t>
+  </si>
+  <si>
+    <t>04/11/1978</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>Dylan</t>
+  </si>
+  <si>
+    <t>diam.Pellentesque@euismodenim.org</t>
+  </si>
+  <si>
+    <t>26/07/1994</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>dui.nec.tempus@parturientmontesnascetur.com</t>
+  </si>
+  <si>
+    <t>21/05/1975</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Salvador</t>
+  </si>
+  <si>
+    <t>eget.metus.In@apurusDuis.org</t>
+  </si>
+  <si>
+    <t>17/04/1988</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>Cyrus</t>
+  </si>
+  <si>
+    <t>Donec@imperdietullamcorper.org</t>
+  </si>
+  <si>
+    <t>31/12/1971</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Kirsten</t>
+  </si>
+  <si>
+    <t>nunc.interdum.feugiat@augue.ca</t>
+  </si>
+  <si>
+    <t>31/07/1998</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Keefe</t>
+  </si>
+  <si>
+    <t>dapibus@CurabiturmassaVestibulum.ca</t>
+  </si>
+  <si>
+    <t>26/06/1974</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Preston</t>
+  </si>
+  <si>
+    <t>nibh.vulputate@eget.co.uk</t>
+  </si>
+  <si>
+    <t>14/12/1995</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>Morbi@Aliquamfringilla.org</t>
+  </si>
+  <si>
+    <t>20/10/1972</t>
+  </si>
+  <si>
+    <t>Caleb</t>
+  </si>
+  <si>
+    <t>Quisque.tincidunt@Quisqueac.ca</t>
+  </si>
+  <si>
+    <t>03/01/1983</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>nunc@sem.ca</t>
+  </si>
+  <si>
+    <t>13/01/2002</t>
+  </si>
+  <si>
+    <t>Iran</t>
+  </si>
+  <si>
+    <t>Aidan</t>
+  </si>
+  <si>
+    <t>ac@velmaurisInteger.org</t>
+  </si>
+  <si>
+    <t>11/03/1970</t>
+  </si>
+  <si>
+    <t>Macedonia</t>
+  </si>
+  <si>
+    <t>Celeste</t>
+  </si>
+  <si>
+    <t>ac.fermentum.vel@urnaconvallis.net</t>
+  </si>
+  <si>
+    <t>30/05/1970</t>
+  </si>
+  <si>
+    <t>Lucian</t>
+  </si>
+  <si>
+    <t>nec.malesuada.ut@diamPellentesque.ca</t>
+  </si>
+  <si>
+    <t>22/02/1996</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Kelsie</t>
+  </si>
+  <si>
+    <t>et.commodo@Nulladignissim.ca</t>
+  </si>
+  <si>
+    <t>15/06/1995</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Kaden</t>
+  </si>
+  <si>
+    <t>et.malesuada.fames@Curabiturvellectus.com</t>
+  </si>
+  <si>
+    <t>16/06/1973</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Athena</t>
+  </si>
+  <si>
+    <t>vitae.nibh.Donec@rhoncusNullamvelit.org</t>
+  </si>
+  <si>
+    <t>27/05/1988</t>
+  </si>
+  <si>
+    <t>Brianna</t>
+  </si>
+  <si>
+    <t>Ut@gravidamauris.net</t>
+  </si>
+  <si>
+    <t>06/12/1990</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Julian</t>
+  </si>
+  <si>
+    <t>vel.venenatis@aliquetmetus.org</t>
+  </si>
+  <si>
+    <t>06/11/1995</t>
+  </si>
+  <si>
+    <t>Niue</t>
+  </si>
+  <si>
+    <t>Graham</t>
+  </si>
+  <si>
+    <t>eget.lacus.Mauris@Curabitursed.co.uk</t>
+  </si>
+  <si>
+    <t>12/03/1975</t>
+  </si>
+  <si>
+    <t>Hop</t>
+  </si>
+  <si>
+    <t>eu@tempus.edu</t>
+  </si>
+  <si>
+    <t>16/04/1979</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Veronica</t>
+  </si>
+  <si>
+    <t>sed@ultricesposuerecubilia.edu</t>
+  </si>
+  <si>
+    <t>28/07/1971</t>
+  </si>
+  <si>
+    <t>Turks and Caicos Islands</t>
+  </si>
+  <si>
+    <t>egestas.rhoncus@luctus.co.uk</t>
+  </si>
+  <si>
+    <t>14/04/1981</t>
+  </si>
+  <si>
+    <t>Kiona</t>
+  </si>
+  <si>
+    <t>velit.Pellentesque.ultricies@Phasellus.org</t>
+  </si>
+  <si>
+    <t>12/09/1977</t>
+  </si>
+  <si>
+    <t>Côte D'Ivoire (Ivory Coast)</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>vel@vestibulumMaurismagna.co.uk</t>
+  </si>
+  <si>
+    <t>18/06/1985</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Kaye</t>
+  </si>
+  <si>
+    <t>natoque.penatibus.et@purusgravida.co.uk</t>
+  </si>
+  <si>
+    <t>23/01/1995</t>
+  </si>
+  <si>
+    <t>Emerson</t>
+  </si>
+  <si>
+    <t>eget.mollis.lectus@nonjustoProin.edu</t>
+  </si>
+  <si>
+    <t>26/11/1987</t>
+  </si>
+  <si>
+    <t>British Indian Ocean Territory</t>
+  </si>
+  <si>
+    <t>Ila</t>
+  </si>
+  <si>
+    <t>pellentesque.eget.dictum@Proin.co.uk</t>
+  </si>
+  <si>
+    <t>18/01/1980</t>
+  </si>
+  <si>
+    <t>Åland Islands</t>
+  </si>
+  <si>
+    <t>Hilel</t>
+  </si>
+  <si>
+    <t>in.faucibus.orci@aliquetmetus.co.uk</t>
+  </si>
+  <si>
+    <t>08/06/1976</t>
+  </si>
+  <si>
+    <t>Blake</t>
+  </si>
+  <si>
+    <t>mauris.ipsum@nuncestmollis.ca</t>
+  </si>
+  <si>
+    <t>01/12/1983</t>
+  </si>
+  <si>
+    <t>Guadeloupe</t>
+  </si>
+  <si>
+    <t>Orla</t>
+  </si>
+  <si>
+    <t>mollis@parturientmontes.com</t>
+  </si>
+  <si>
+    <t>11/01/2002</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Shoshana</t>
+  </si>
+  <si>
+    <t>diam.Proin@egestasblanditNam.net</t>
+  </si>
+  <si>
+    <t>20/07/1976</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>Nadine</t>
+  </si>
+  <si>
+    <t>elit@acmattisornare.co.uk</t>
+  </si>
+  <si>
+    <t>11/11/1987</t>
+  </si>
+  <si>
+    <t>Kevyn</t>
+  </si>
+  <si>
+    <t>erat@tellussem.ca</t>
+  </si>
+  <si>
+    <t>06/09/1983</t>
+  </si>
+  <si>
+    <t>Korea, North</t>
+  </si>
+  <si>
+    <t>Brenna</t>
+  </si>
+  <si>
+    <t>amet@risusDonec.ca</t>
+  </si>
+  <si>
+    <t>26/03/1982</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
+  </si>
+  <si>
+    <t>Levi</t>
+  </si>
+  <si>
+    <t>amet.ultricies@necurnasuscipit.edu</t>
+  </si>
+  <si>
+    <t>28/03/1993</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Lilah</t>
+  </si>
+  <si>
+    <t>Mauris@ligula.org</t>
+  </si>
+  <si>
+    <t>18/09/1995</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Thor</t>
+  </si>
+  <si>
+    <t>nibh.Quisque.nonummy@Proinnisl.co.uk</t>
+  </si>
+  <si>
+    <t>06/07/1992</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Lillith</t>
+  </si>
+  <si>
+    <t>nisl.arcu.iaculis@nonegestasa.com</t>
+  </si>
+  <si>
+    <t>01/11/1992</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Nolan</t>
+  </si>
+  <si>
+    <t>Sed.id.risus@laciniaorci.net</t>
+  </si>
+  <si>
+    <t>01/11/1976</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Tatiana</t>
+  </si>
+  <si>
+    <t>mi@fringilla.edu</t>
+  </si>
+  <si>
+    <t>08/05/1972</t>
+  </si>
+  <si>
+    <t>Serena</t>
+  </si>
+  <si>
+    <t>nulla.vulputate@Vivamus.ca</t>
+  </si>
+  <si>
+    <t>25/05/1978</t>
+  </si>
+  <si>
+    <t>Sydnee</t>
+  </si>
+  <si>
+    <t>vel.mauris@nonsapienmolestie.ca</t>
+  </si>
+  <si>
+    <t>14/03/1986</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Chase</t>
+  </si>
+  <si>
+    <t>Fusce.aliquet.magna@Proinnisl.org</t>
+  </si>
+  <si>
+    <t>04/01/1990</t>
+  </si>
+  <si>
+    <t>Xander</t>
+  </si>
+  <si>
+    <t>quis@ultriciesligula.edu</t>
+  </si>
+  <si>
+    <t>22/08/1976</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>tempus.lorem@nibhAliquamornare.edu</t>
+  </si>
+  <si>
+    <t>15/01/1988</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Quin</t>
+  </si>
+  <si>
+    <t>Curabitur.egestas.nunc@venenatislacusEtiam.net</t>
+  </si>
+  <si>
+    <t>03/01/1981</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Ella</t>
+  </si>
+  <si>
+    <t>diam@Vivamusmolestie.ca</t>
+  </si>
+  <si>
+    <t>21/07/1997</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Nigel</t>
+  </si>
+  <si>
+    <t>tristique@atpede.net</t>
+  </si>
+  <si>
+    <t>21/02/1974</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>enim.consequat.purus@aliquetmolestie.edu</t>
+  </si>
+  <si>
+    <t>17/10/1972</t>
+  </si>
+  <si>
+    <t>Wallis and Futuna</t>
+  </si>
+  <si>
+    <t>Cameran</t>
+  </si>
+  <si>
+    <t>elit.Etiam@faucibusMorbi.org</t>
+  </si>
+  <si>
+    <t>21/07/1989</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Mufutau</t>
+  </si>
+  <si>
+    <t>adipiscing@neque.co.uk</t>
+  </si>
+  <si>
+    <t>30/08/1978</t>
+  </si>
+  <si>
+    <t>Activities</t>
+  </si>
+  <si>
+    <t>Registered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gisela   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Echo</t>
+  </si>
+  <si>
     <t>Solomon</t>
-  </si>
-  <si>
-    <t>malesuada.fames.ac@Maurisnondui.edu</t>
-  </si>
-  <si>
-    <t>29/11/1986</t>
-  </si>
-  <si>
-    <t>Holy See (Vatican City State)</t>
-  </si>
-  <si>
-    <t>Quamar</t>
-  </si>
-  <si>
-    <t>gravida.non@Aliquamornare.edu</t>
-  </si>
-  <si>
-    <t>27/07/1994</t>
-  </si>
-  <si>
-    <t>Mali</t>
-  </si>
-  <si>
-    <t>Lacota</t>
-  </si>
-  <si>
-    <t>facilisis@Proinnon.com</t>
-  </si>
-  <si>
-    <t>29/05/1984</t>
-  </si>
-  <si>
-    <t>Lithuania</t>
-  </si>
-  <si>
-    <t>Sylvester</t>
-  </si>
-  <si>
-    <t>sagittis.lobortis.mauris@loremsitamet.org</t>
-  </si>
-  <si>
-    <t>02/03/1979</t>
-  </si>
-  <si>
-    <t>Sloane</t>
-  </si>
-  <si>
-    <t>vulputate@senectus.com</t>
-  </si>
-  <si>
-    <t>06/05/1998</t>
-  </si>
-  <si>
-    <t>Mauritius</t>
-  </si>
-  <si>
-    <t>Arthur</t>
-  </si>
-  <si>
-    <t>cursus.purus@risusaultricies.edu</t>
-  </si>
-  <si>
-    <t>14/10/1997</t>
-  </si>
-  <si>
-    <t>Tonga</t>
-  </si>
-  <si>
-    <t>Hakeem</t>
-  </si>
-  <si>
-    <t>nec.luctus@hendreritidante.ca</t>
-  </si>
-  <si>
-    <t>10/02/1972</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Fritz</t>
-  </si>
-  <si>
-    <t>molestie.Sed.id@adipiscingelitCurabitur.org</t>
-  </si>
-  <si>
-    <t>21/05/2002</t>
-  </si>
-  <si>
-    <t>Niger</t>
-  </si>
-  <si>
-    <t>Callum</t>
-  </si>
-  <si>
-    <t>fringilla.cursus.purus@ultrices.co.uk</t>
-  </si>
-  <si>
-    <t>08/07/1991</t>
-  </si>
-  <si>
-    <t>Rinah</t>
-  </si>
-  <si>
-    <t>morbi@lacuspedesagittis.edu</t>
-  </si>
-  <si>
-    <t>10/03/1998</t>
-  </si>
-  <si>
-    <t>Honduras</t>
-  </si>
-  <si>
-    <t>interdum@infelis.net</t>
-  </si>
-  <si>
-    <t>16/09/1996</t>
-  </si>
-  <si>
-    <t>France</t>
-  </si>
-  <si>
-    <t>Demetria</t>
-  </si>
-  <si>
-    <t>Donec@pharetraQuisqueac.org</t>
-  </si>
-  <si>
-    <t>08/07/1984</t>
-  </si>
-  <si>
-    <t>Western Sahara</t>
-  </si>
-  <si>
-    <t>Sean</t>
-  </si>
-  <si>
-    <t>sociosqu.ad@lectusconvallisest.ca</t>
-  </si>
-  <si>
-    <t>27/11/1987</t>
-  </si>
-  <si>
-    <t>Ghana</t>
-  </si>
-  <si>
-    <t>Cole</t>
-  </si>
-  <si>
-    <t>amet.luctus.vulputate@non.co.uk</t>
-  </si>
-  <si>
-    <t>22/04/1989</t>
-  </si>
-  <si>
-    <t>Saint Lucia</t>
-  </si>
-  <si>
-    <t>Oscar</t>
-  </si>
-  <si>
-    <t>mattis.ornare.lectus@IncondimentumDonec.net</t>
-  </si>
-  <si>
-    <t>17/01/1980</t>
-  </si>
-  <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Kaitlin</t>
-  </si>
-  <si>
-    <t>luctus@metusurnaconvallis.ca</t>
-  </si>
-  <si>
-    <t>10/06/1976</t>
-  </si>
-  <si>
-    <t>Raymond</t>
-  </si>
-  <si>
-    <t>Quisque@Donecdignissimmagna.ca</t>
-  </si>
-  <si>
-    <t>26/10/2001</t>
-  </si>
-  <si>
-    <t>Saint Martin</t>
-  </si>
-  <si>
-    <t>Allegra</t>
-  </si>
-  <si>
-    <t>blandit.Nam.nulla@aliquetmetus.ca</t>
-  </si>
-  <si>
-    <t>11/11/1994</t>
-  </si>
-  <si>
-    <t>Papua New Guinea</t>
-  </si>
-  <si>
-    <t>Elliott</t>
-  </si>
-  <si>
-    <t>orci@feugiat.com</t>
-  </si>
-  <si>
-    <t>04/11/1978</t>
-  </si>
-  <si>
-    <t>Sierra Leone</t>
-  </si>
-  <si>
-    <t>Dylan</t>
-  </si>
-  <si>
-    <t>diam.Pellentesque@euismodenim.org</t>
-  </si>
-  <si>
-    <t>26/07/1994</t>
-  </si>
-  <si>
-    <t>Malta</t>
-  </si>
-  <si>
-    <t>Victoria</t>
-  </si>
-  <si>
-    <t>dui.nec.tempus@parturientmontesnascetur.com</t>
-  </si>
-  <si>
-    <t>21/05/1975</t>
-  </si>
-  <si>
-    <t>Iceland</t>
-  </si>
-  <si>
-    <t>Salvador</t>
-  </si>
-  <si>
-    <t>eget.metus.In@apurusDuis.org</t>
-  </si>
-  <si>
-    <t>17/04/1988</t>
-  </si>
-  <si>
-    <t>Namibia</t>
-  </si>
-  <si>
-    <t>Cyrus</t>
-  </si>
-  <si>
-    <t>Donec@imperdietullamcorper.org</t>
-  </si>
-  <si>
-    <t>31/12/1971</t>
-  </si>
-  <si>
-    <t>Turkmenistan</t>
-  </si>
-  <si>
-    <t>Kirsten</t>
-  </si>
-  <si>
-    <t>nunc.interdum.feugiat@augue.ca</t>
-  </si>
-  <si>
-    <t>31/07/1998</t>
-  </si>
-  <si>
-    <t>Monaco</t>
-  </si>
-  <si>
-    <t>Keefe</t>
-  </si>
-  <si>
-    <t>dapibus@CurabiturmassaVestibulum.ca</t>
-  </si>
-  <si>
-    <t>26/06/1974</t>
-  </si>
-  <si>
-    <t>Kazakhstan</t>
-  </si>
-  <si>
-    <t>Preston</t>
-  </si>
-  <si>
-    <t>nibh.vulputate@eget.co.uk</t>
-  </si>
-  <si>
-    <t>14/12/1995</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Craig</t>
-  </si>
-  <si>
-    <t>Morbi@Aliquamfringilla.org</t>
-  </si>
-  <si>
-    <t>20/10/1972</t>
-  </si>
-  <si>
-    <t>Caleb</t>
-  </si>
-  <si>
-    <t>Quisque.tincidunt@Quisqueac.ca</t>
-  </si>
-  <si>
-    <t>03/01/1983</t>
-  </si>
-  <si>
-    <t>Vanuatu</t>
-  </si>
-  <si>
-    <t>Benjamin</t>
-  </si>
-  <si>
-    <t>nunc@sem.ca</t>
-  </si>
-  <si>
-    <t>13/01/2002</t>
-  </si>
-  <si>
-    <t>Iran</t>
-  </si>
-  <si>
-    <t>Aidan</t>
-  </si>
-  <si>
-    <t>ac@velmaurisInteger.org</t>
-  </si>
-  <si>
-    <t>11/03/1970</t>
-  </si>
-  <si>
-    <t>Macedonia</t>
-  </si>
-  <si>
-    <t>Celeste</t>
-  </si>
-  <si>
-    <t>ac.fermentum.vel@urnaconvallis.net</t>
-  </si>
-  <si>
-    <t>30/05/1970</t>
-  </si>
-  <si>
-    <t>Lucian</t>
-  </si>
-  <si>
-    <t>nec.malesuada.ut@diamPellentesque.ca</t>
-  </si>
-  <si>
-    <t>22/02/1996</t>
-  </si>
-  <si>
-    <t>New Zealand</t>
-  </si>
-  <si>
-    <t>Kelsie</t>
-  </si>
-  <si>
-    <t>et.commodo@Nulladignissim.ca</t>
-  </si>
-  <si>
-    <t>15/06/1995</t>
-  </si>
-  <si>
-    <t>Bahrain</t>
-  </si>
-  <si>
-    <t>Kaden</t>
-  </si>
-  <si>
-    <t>et.malesuada.fames@Curabiturvellectus.com</t>
-  </si>
-  <si>
-    <t>16/06/1973</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>Athena</t>
-  </si>
-  <si>
-    <t>vitae.nibh.Donec@rhoncusNullamvelit.org</t>
-  </si>
-  <si>
-    <t>27/05/1988</t>
-  </si>
-  <si>
-    <t>Brianna</t>
-  </si>
-  <si>
-    <t>Ut@gravidamauris.net</t>
-  </si>
-  <si>
-    <t>06/12/1990</t>
-  </si>
-  <si>
-    <t>Lebanon</t>
-  </si>
-  <si>
-    <t>Julian</t>
-  </si>
-  <si>
-    <t>vel.venenatis@aliquetmetus.org</t>
-  </si>
-  <si>
-    <t>06/11/1995</t>
-  </si>
-  <si>
-    <t>Niue</t>
-  </si>
-  <si>
-    <t>Graham</t>
-  </si>
-  <si>
-    <t>eget.lacus.Mauris@Curabitursed.co.uk</t>
-  </si>
-  <si>
-    <t>12/03/1975</t>
-  </si>
-  <si>
-    <t>Hop</t>
-  </si>
-  <si>
-    <t>eu@tempus.edu</t>
-  </si>
-  <si>
-    <t>16/04/1979</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
-    <t>Veronica</t>
-  </si>
-  <si>
-    <t>sed@ultricesposuerecubilia.edu</t>
-  </si>
-  <si>
-    <t>28/07/1971</t>
-  </si>
-  <si>
-    <t>Turks and Caicos Islands</t>
-  </si>
-  <si>
-    <t>egestas.rhoncus@luctus.co.uk</t>
-  </si>
-  <si>
-    <t>14/04/1981</t>
-  </si>
-  <si>
-    <t>Kiona</t>
-  </si>
-  <si>
-    <t>velit.Pellentesque.ultricies@Phasellus.org</t>
-  </si>
-  <si>
-    <t>12/09/1977</t>
-  </si>
-  <si>
-    <t>Côte D'Ivoire (Ivory Coast)</t>
-  </si>
-  <si>
-    <t>Oliver</t>
-  </si>
-  <si>
-    <t>vel@vestibulumMaurismagna.co.uk</t>
-  </si>
-  <si>
-    <t>18/06/1985</t>
-  </si>
-  <si>
-    <t>Mongolia</t>
-  </si>
-  <si>
-    <t>Kaye</t>
-  </si>
-  <si>
-    <t>natoque.penatibus.et@purusgravida.co.uk</t>
-  </si>
-  <si>
-    <t>23/01/1995</t>
-  </si>
-  <si>
-    <t>Emerson</t>
-  </si>
-  <si>
-    <t>eget.mollis.lectus@nonjustoProin.edu</t>
-  </si>
-  <si>
-    <t>26/11/1987</t>
-  </si>
-  <si>
-    <t>British Indian Ocean Territory</t>
-  </si>
-  <si>
-    <t>Ila</t>
-  </si>
-  <si>
-    <t>pellentesque.eget.dictum@Proin.co.uk</t>
-  </si>
-  <si>
-    <t>18/01/1980</t>
-  </si>
-  <si>
-    <t>Åland Islands</t>
-  </si>
-  <si>
-    <t>Hilel</t>
-  </si>
-  <si>
-    <t>in.faucibus.orci@aliquetmetus.co.uk</t>
-  </si>
-  <si>
-    <t>08/06/1976</t>
-  </si>
-  <si>
-    <t>Blake</t>
-  </si>
-  <si>
-    <t>mauris.ipsum@nuncestmollis.ca</t>
-  </si>
-  <si>
-    <t>01/12/1983</t>
-  </si>
-  <si>
-    <t>Guadeloupe</t>
-  </si>
-  <si>
-    <t>Orla</t>
-  </si>
-  <si>
-    <t>mollis@parturientmontes.com</t>
-  </si>
-  <si>
-    <t>11/01/2002</t>
-  </si>
-  <si>
-    <t>Turkey</t>
-  </si>
-  <si>
-    <t>Shoshana</t>
-  </si>
-  <si>
-    <t>diam.Proin@egestasblanditNam.net</t>
-  </si>
-  <si>
-    <t>20/07/1976</t>
-  </si>
-  <si>
-    <t>Samoa</t>
-  </si>
-  <si>
-    <t>Nadine</t>
-  </si>
-  <si>
-    <t>elit@acmattisornare.co.uk</t>
-  </si>
-  <si>
-    <t>11/11/1987</t>
-  </si>
-  <si>
-    <t>Kevyn</t>
-  </si>
-  <si>
-    <t>erat@tellussem.ca</t>
-  </si>
-  <si>
-    <t>06/09/1983</t>
-  </si>
-  <si>
-    <t>Korea, North</t>
-  </si>
-  <si>
-    <t>Brenna</t>
-  </si>
-  <si>
-    <t>amet@risusDonec.ca</t>
-  </si>
-  <si>
-    <t>26/03/1982</t>
-  </si>
-  <si>
-    <t>Bolivia</t>
-  </si>
-  <si>
-    <t>Levi</t>
-  </si>
-  <si>
-    <t>amet.ultricies@necurnasuscipit.edu</t>
-  </si>
-  <si>
-    <t>28/03/1993</t>
-  </si>
-  <si>
-    <t>Hungary</t>
-  </si>
-  <si>
-    <t>Lilah</t>
-  </si>
-  <si>
-    <t>Mauris@ligula.org</t>
-  </si>
-  <si>
-    <t>18/09/1995</t>
-  </si>
-  <si>
-    <t>South Africa</t>
-  </si>
-  <si>
-    <t>Thor</t>
-  </si>
-  <si>
-    <t>nibh.Quisque.nonummy@Proinnisl.co.uk</t>
-  </si>
-  <si>
-    <t>06/07/1992</t>
-  </si>
-  <si>
-    <t>Serbia</t>
-  </si>
-  <si>
-    <t>Lillith</t>
-  </si>
-  <si>
-    <t>nisl.arcu.iaculis@nonegestasa.com</t>
-  </si>
-  <si>
-    <t>01/11/1992</t>
-  </si>
-  <si>
-    <t>Costa Rica</t>
-  </si>
-  <si>
-    <t>Nolan</t>
-  </si>
-  <si>
-    <t>Sed.id.risus@laciniaorci.net</t>
-  </si>
-  <si>
-    <t>01/11/1976</t>
-  </si>
-  <si>
-    <t>Algeria</t>
-  </si>
-  <si>
-    <t>Tatiana</t>
-  </si>
-  <si>
-    <t>mi@fringilla.edu</t>
-  </si>
-  <si>
-    <t>08/05/1972</t>
-  </si>
-  <si>
-    <t>Serena</t>
-  </si>
-  <si>
-    <t>nulla.vulputate@Vivamus.ca</t>
-  </si>
-  <si>
-    <t>25/05/1978</t>
-  </si>
-  <si>
-    <t>Sydnee</t>
-  </si>
-  <si>
-    <t>vel.mauris@nonsapienmolestie.ca</t>
-  </si>
-  <si>
-    <t>14/03/1986</t>
-  </si>
-  <si>
-    <t>United Arab Emirates</t>
-  </si>
-  <si>
-    <t>Chase</t>
-  </si>
-  <si>
-    <t>Fusce.aliquet.magna@Proinnisl.org</t>
-  </si>
-  <si>
-    <t>04/01/1990</t>
-  </si>
-  <si>
-    <t>Xander</t>
-  </si>
-  <si>
-    <t>quis@ultriciesligula.edu</t>
-  </si>
-  <si>
-    <t>22/08/1976</t>
-  </si>
-  <si>
-    <t>Zambia</t>
-  </si>
-  <si>
-    <t>Nathan</t>
-  </si>
-  <si>
-    <t>tempus.lorem@nibhAliquamornare.edu</t>
-  </si>
-  <si>
-    <t>15/01/1988</t>
-  </si>
-  <si>
-    <t>Bahamas</t>
-  </si>
-  <si>
-    <t>Quin</t>
-  </si>
-  <si>
-    <t>Curabitur.egestas.nunc@venenatislacusEtiam.net</t>
-  </si>
-  <si>
-    <t>03/01/1981</t>
-  </si>
-  <si>
-    <t>Azerbaijan</t>
-  </si>
-  <si>
-    <t>Ella</t>
-  </si>
-  <si>
-    <t>diam@Vivamusmolestie.ca</t>
-  </si>
-  <si>
-    <t>21/07/1997</t>
-  </si>
-  <si>
-    <t>Belize</t>
-  </si>
-  <si>
-    <t>Nigel</t>
-  </si>
-  <si>
-    <t>tristique@atpede.net</t>
-  </si>
-  <si>
-    <t>21/02/1974</t>
-  </si>
-  <si>
-    <t>San Marino</t>
-  </si>
-  <si>
-    <t>Jessica</t>
-  </si>
-  <si>
-    <t>enim.consequat.purus@aliquetmolestie.edu</t>
-  </si>
-  <si>
-    <t>17/10/1972</t>
-  </si>
-  <si>
-    <t>Wallis and Futuna</t>
-  </si>
-  <si>
-    <t>Cameran</t>
-  </si>
-  <si>
-    <t>elit.Etiam@faucibusMorbi.org</t>
-  </si>
-  <si>
-    <t>21/07/1989</t>
-  </si>
-  <si>
-    <t>Ukraine</t>
-  </si>
-  <si>
-    <t>Mufutau</t>
-  </si>
-  <si>
-    <t>adipiscing@neque.co.uk</t>
-  </si>
-  <si>
-    <t>30/08/1978</t>
-  </si>
-  <si>
-    <t>Activities</t>
-  </si>
-  <si>
-    <t>Registered</t>
   </si>
 </sst>
 </file>
@@ -1540,7 +1543,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1564,10 +1569,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2172,16 +2177,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>389</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>125</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D32" t="s">
-        <v>127</v>
       </c>
       <c r="E32">
         <v>10</v>
@@ -2192,16 +2194,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>129</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="D33" t="s">
-        <v>131</v>
       </c>
       <c r="E33">
         <v>4</v>
@@ -2212,16 +2214,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>130</v>
+      </c>
+      <c r="B34" t="s">
+        <v>131</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>133</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D34" t="s">
-        <v>135</v>
       </c>
       <c r="E34">
         <v>11</v>
@@ -2232,13 +2234,13 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="B35" t="s">
-        <v>137</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="D35" t="s">
         <v>15</v>
@@ -2252,16 +2254,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>137</v>
+      </c>
+      <c r="B36" t="s">
+        <v>138</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>140</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D36" t="s">
-        <v>142</v>
       </c>
       <c r="E36">
         <v>13</v>
@@ -2272,16 +2274,16 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B37" t="s">
+      <c r="D37" t="s">
         <v>144</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D37" t="s">
-        <v>146</v>
       </c>
       <c r="E37">
         <v>6</v>
@@ -2292,16 +2294,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" t="s">
         <v>148</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D38" t="s">
-        <v>150</v>
       </c>
       <c r="E38">
         <v>5</v>
@@ -2312,16 +2314,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>149</v>
+      </c>
+      <c r="B39" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
         <v>152</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D39" t="s">
-        <v>154</v>
       </c>
       <c r="E39">
         <v>17</v>
@@ -2332,13 +2334,13 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" t="s">
+        <v>154</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B40" t="s">
-        <v>156</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>157</v>
       </c>
       <c r="D40" t="s">
         <v>39</v>
@@ -2352,16 +2354,16 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>156</v>
+      </c>
+      <c r="B41" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>159</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D41" t="s">
-        <v>161</v>
       </c>
       <c r="E41">
         <v>16</v>
@@ -2372,16 +2374,16 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B42" t="s">
+        <v>160</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" t="s">
         <v>162</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="D42" t="s">
-        <v>164</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -2392,16 +2394,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>163</v>
+      </c>
+      <c r="B43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
         <v>166</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="D43" t="s">
-        <v>168</v>
       </c>
       <c r="E43">
         <v>4</v>
@@ -2412,16 +2414,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>167</v>
+      </c>
+      <c r="B44" t="s">
+        <v>168</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="B44" t="s">
+      <c r="D44" t="s">
         <v>170</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D44" t="s">
-        <v>172</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -2432,16 +2434,16 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>171</v>
+      </c>
+      <c r="B45" t="s">
+        <v>172</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D45" t="s">
         <v>174</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D45" t="s">
-        <v>176</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -2452,16 +2454,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>175</v>
+      </c>
+      <c r="B46" t="s">
+        <v>176</v>
+      </c>
+      <c r="C46" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>178</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="D46" t="s">
-        <v>180</v>
       </c>
       <c r="E46">
         <v>6</v>
@@ -2472,16 +2474,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>179</v>
+      </c>
+      <c r="B47" t="s">
+        <v>180</v>
+      </c>
+      <c r="C47" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B47" t="s">
-        <v>182</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="D47" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E47">
         <v>20</v>
@@ -2492,16 +2494,16 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>182</v>
+      </c>
+      <c r="B48" t="s">
+        <v>183</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" t="s">
         <v>185</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D48" t="s">
-        <v>187</v>
       </c>
       <c r="E48">
         <v>1</v>
@@ -2512,16 +2514,16 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>186</v>
+      </c>
+      <c r="B49" t="s">
+        <v>187</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B49" t="s">
+      <c r="D49" t="s">
         <v>189</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D49" t="s">
-        <v>191</v>
       </c>
       <c r="E49">
         <v>19</v>
@@ -2532,16 +2534,16 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>190</v>
+      </c>
+      <c r="B50" t="s">
+        <v>191</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B50" t="s">
+      <c r="D50" t="s">
         <v>193</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D50" t="s">
-        <v>195</v>
       </c>
       <c r="E50">
         <v>2</v>
@@ -2552,16 +2554,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>194</v>
+      </c>
+      <c r="B51" t="s">
+        <v>195</v>
+      </c>
+      <c r="C51" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="B51" t="s">
+      <c r="D51" t="s">
         <v>197</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D51" t="s">
-        <v>199</v>
       </c>
       <c r="E51">
         <v>15</v>
@@ -2572,16 +2574,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>198</v>
+      </c>
+      <c r="B52" t="s">
+        <v>199</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
         <v>201</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D52" t="s">
-        <v>203</v>
       </c>
       <c r="E52">
         <v>20</v>
@@ -2592,16 +2594,16 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>202</v>
+      </c>
+      <c r="B53" t="s">
+        <v>203</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B53" t="s">
+      <c r="D53" t="s">
         <v>205</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D53" t="s">
-        <v>207</v>
       </c>
       <c r="E53">
         <v>10</v>
@@ -2612,16 +2614,16 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>206</v>
+      </c>
+      <c r="B54" t="s">
+        <v>207</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>209</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="D54" t="s">
-        <v>211</v>
       </c>
       <c r="E54">
         <v>17</v>
@@ -2632,16 +2634,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>210</v>
+      </c>
+      <c r="B55" t="s">
+        <v>211</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B55" t="s">
+      <c r="D55" t="s">
         <v>213</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D55" t="s">
-        <v>215</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -2652,16 +2654,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>214</v>
+      </c>
+      <c r="B56" t="s">
+        <v>215</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
         <v>217</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D56" t="s">
-        <v>219</v>
       </c>
       <c r="E56">
         <v>11</v>
@@ -2672,16 +2674,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>218</v>
+      </c>
+      <c r="B57" t="s">
+        <v>219</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="B57" t="s">
+      <c r="D57" t="s">
         <v>221</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D57" t="s">
-        <v>223</v>
       </c>
       <c r="E57">
         <v>13</v>
@@ -2692,16 +2694,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>222</v>
+      </c>
+      <c r="B58" t="s">
+        <v>223</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="B58" t="s">
-        <v>225</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>226</v>
-      </c>
       <c r="D58" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E58">
         <v>1</v>
@@ -2712,16 +2714,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>225</v>
+      </c>
+      <c r="B59" t="s">
+        <v>226</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
         <v>228</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D59" t="s">
-        <v>230</v>
       </c>
       <c r="E59">
         <v>9</v>
@@ -2732,16 +2734,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>229</v>
+      </c>
+      <c r="B60" t="s">
+        <v>230</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="B60" t="s">
+      <c r="D60" t="s">
         <v>232</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="D60" t="s">
-        <v>234</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -2752,16 +2754,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>233</v>
+      </c>
+      <c r="B61" t="s">
+        <v>234</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="B61" t="s">
+      <c r="D61" t="s">
         <v>236</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D61" t="s">
-        <v>238</v>
       </c>
       <c r="E61">
         <v>3</v>
@@ -2772,13 +2774,13 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>237</v>
+      </c>
+      <c r="B62" t="s">
+        <v>238</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>239</v>
-      </c>
-      <c r="B62" t="s">
-        <v>240</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>241</v>
       </c>
       <c r="D62" t="s">
         <v>95</v>
@@ -2792,16 +2794,16 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>240</v>
+      </c>
+      <c r="B63" t="s">
+        <v>241</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" t="s">
         <v>243</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D63" t="s">
-        <v>245</v>
       </c>
       <c r="E63">
         <v>8</v>
@@ -2812,16 +2814,16 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>244</v>
+      </c>
+      <c r="B64" t="s">
+        <v>245</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B64" t="s">
+      <c r="D64" t="s">
         <v>247</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D64" t="s">
-        <v>249</v>
       </c>
       <c r="E64">
         <v>7</v>
@@ -2832,16 +2834,16 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>248</v>
+      </c>
+      <c r="B65" t="s">
+        <v>249</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" t="s">
         <v>251</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="D65" t="s">
-        <v>253</v>
       </c>
       <c r="E65">
         <v>1</v>
@@ -2852,16 +2854,16 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>252</v>
+      </c>
+      <c r="B66" t="s">
+        <v>253</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B66" t="s">
-        <v>255</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>256</v>
-      </c>
       <c r="D66" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E66">
         <v>7</v>
@@ -2872,16 +2874,16 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>255</v>
+      </c>
+      <c r="B67" t="s">
+        <v>256</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B67" t="s">
+      <c r="D67" t="s">
         <v>258</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="D67" t="s">
-        <v>260</v>
       </c>
       <c r="E67">
         <v>17</v>
@@ -2892,16 +2894,16 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>259</v>
+      </c>
+      <c r="B68" t="s">
+        <v>260</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B68" t="s">
+      <c r="D68" t="s">
         <v>262</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>263</v>
-      </c>
-      <c r="D68" t="s">
-        <v>264</v>
       </c>
       <c r="E68">
         <v>6</v>
@@ -2912,16 +2914,16 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>263</v>
+      </c>
+      <c r="B69" t="s">
+        <v>264</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B69" t="s">
-        <v>266</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="D69" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E69">
         <v>20</v>
@@ -2932,16 +2934,16 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>266</v>
+      </c>
+      <c r="B70" t="s">
+        <v>267</v>
+      </c>
+      <c r="C70" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B70" t="s">
+      <c r="D70" t="s">
         <v>269</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D70" t="s">
-        <v>271</v>
       </c>
       <c r="E70">
         <v>11</v>
@@ -2952,16 +2954,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>270</v>
+      </c>
+      <c r="B71" t="s">
+        <v>271</v>
+      </c>
+      <c r="C71" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B71" t="s">
+      <c r="D71" t="s">
         <v>273</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="D71" t="s">
-        <v>275</v>
       </c>
       <c r="E71">
         <v>1</v>
@@ -2975,13 +2977,13 @@
         <v>40</v>
       </c>
       <c r="B72" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D72" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E72">
         <v>13</v>
@@ -2992,16 +2994,16 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>276</v>
+      </c>
+      <c r="B73" t="s">
+        <v>277</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D73" t="s">
         <v>279</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="D73" t="s">
-        <v>281</v>
       </c>
       <c r="E73">
         <v>16</v>
@@ -3012,16 +3014,16 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>280</v>
+      </c>
+      <c r="B74" t="s">
+        <v>281</v>
+      </c>
+      <c r="C74" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B74" t="s">
+      <c r="D74" t="s">
         <v>283</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="D74" t="s">
-        <v>285</v>
       </c>
       <c r="E74">
         <v>10</v>
@@ -3032,16 +3034,16 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>284</v>
+      </c>
+      <c r="B75" t="s">
+        <v>285</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B75" t="s">
-        <v>287</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>288</v>
-      </c>
       <c r="D75" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E75">
         <v>13</v>
@@ -3052,16 +3054,16 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>287</v>
+      </c>
+      <c r="B76" t="s">
+        <v>288</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B76" t="s">
+      <c r="D76" t="s">
         <v>290</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="D76" t="s">
-        <v>292</v>
       </c>
       <c r="E76">
         <v>8</v>
@@ -3072,16 +3074,16 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>291</v>
+      </c>
+      <c r="B77" t="s">
+        <v>292</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B77" t="s">
+      <c r="D77" t="s">
         <v>294</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D77" t="s">
-        <v>296</v>
       </c>
       <c r="E77">
         <v>7</v>
@@ -3092,13 +3094,13 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>295</v>
+      </c>
+      <c r="B78" t="s">
+        <v>296</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>297</v>
-      </c>
-      <c r="B78" t="s">
-        <v>298</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>299</v>
       </c>
       <c r="D78" t="s">
         <v>67</v>
@@ -3112,16 +3114,16 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>298</v>
+      </c>
+      <c r="B79" t="s">
+        <v>299</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
         <v>301</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="D79" t="s">
-        <v>303</v>
       </c>
       <c r="E79">
         <v>13</v>
@@ -3132,16 +3134,16 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>302</v>
+      </c>
+      <c r="B80" t="s">
+        <v>303</v>
+      </c>
+      <c r="C80" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="B80" t="s">
+      <c r="D80" t="s">
         <v>305</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="D80" t="s">
-        <v>307</v>
       </c>
       <c r="E80">
         <v>17</v>
@@ -3152,16 +3154,16 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>306</v>
+      </c>
+      <c r="B81" t="s">
+        <v>307</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>309</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="D81" t="s">
-        <v>311</v>
       </c>
       <c r="E81">
         <v>12</v>
@@ -3172,13 +3174,13 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>310</v>
+      </c>
+      <c r="B82" t="s">
+        <v>311</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="B82" t="s">
-        <v>313</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>314</v>
       </c>
       <c r="D82" t="s">
         <v>27</v>
@@ -3192,16 +3194,16 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>313</v>
+      </c>
+      <c r="B83" t="s">
+        <v>314</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>315</v>
       </c>
-      <c r="B83" t="s">
+      <c r="D83" t="s">
         <v>316</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D83" t="s">
-        <v>318</v>
       </c>
       <c r="E83">
         <v>15</v>
@@ -3212,16 +3214,16 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>317</v>
+      </c>
+      <c r="B84" t="s">
+        <v>318</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B84" t="s">
+      <c r="D84" t="s">
         <v>320</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="D84" t="s">
-        <v>322</v>
       </c>
       <c r="E84">
         <v>19</v>
@@ -3232,16 +3234,16 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>321</v>
+      </c>
+      <c r="B85" t="s">
+        <v>322</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B85" t="s">
+      <c r="D85" t="s">
         <v>324</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="D85" t="s">
-        <v>326</v>
       </c>
       <c r="E85">
         <v>12</v>
@@ -3252,16 +3254,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>325</v>
+      </c>
+      <c r="B86" t="s">
+        <v>326</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="B86" t="s">
+      <c r="D86" t="s">
         <v>328</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="D86" t="s">
-        <v>330</v>
       </c>
       <c r="E86">
         <v>14</v>
@@ -3272,16 +3274,16 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>329</v>
+      </c>
+      <c r="B87" t="s">
+        <v>330</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>331</v>
       </c>
-      <c r="B87" t="s">
+      <c r="D87" t="s">
         <v>332</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="D87" t="s">
-        <v>334</v>
       </c>
       <c r="E87">
         <v>3</v>
@@ -3292,16 +3294,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>333</v>
+      </c>
+      <c r="B88" t="s">
+        <v>334</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B88" t="s">
+      <c r="D88" t="s">
         <v>336</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="D88" t="s">
-        <v>338</v>
       </c>
       <c r="E88">
         <v>2</v>
@@ -3312,16 +3314,16 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>337</v>
+      </c>
+      <c r="B89" t="s">
+        <v>338</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B89" t="s">
+      <c r="D89" t="s">
         <v>340</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D89" t="s">
-        <v>342</v>
       </c>
       <c r="E89">
         <v>2</v>
@@ -3332,13 +3334,13 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>341</v>
+      </c>
+      <c r="B90" t="s">
+        <v>342</v>
+      </c>
+      <c r="C90" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="B90" t="s">
-        <v>344</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>345</v>
       </c>
       <c r="D90" t="s">
         <v>123</v>
@@ -3352,16 +3354,16 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>344</v>
+      </c>
+      <c r="B91" t="s">
+        <v>345</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="B91" t="s">
-        <v>347</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>348</v>
-      </c>
       <c r="D91" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E91">
         <v>19</v>
@@ -3372,16 +3374,16 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>347</v>
+      </c>
+      <c r="B92" t="s">
+        <v>348</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="B92" t="s">
+      <c r="D92" t="s">
         <v>350</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>351</v>
-      </c>
-      <c r="D92" t="s">
-        <v>352</v>
       </c>
       <c r="E92">
         <v>9</v>
@@ -3392,16 +3394,16 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>351</v>
+      </c>
+      <c r="B93" t="s">
+        <v>352</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="B93" t="s">
-        <v>354</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>355</v>
-      </c>
       <c r="D93" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E93">
         <v>10</v>
@@ -3412,16 +3414,16 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>354</v>
+      </c>
+      <c r="B94" t="s">
+        <v>355</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="B94" t="s">
+      <c r="D94" t="s">
         <v>357</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="D94" t="s">
-        <v>359</v>
       </c>
       <c r="E94">
         <v>1</v>
@@ -3432,16 +3434,16 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>358</v>
+      </c>
+      <c r="B95" t="s">
+        <v>359</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="B95" t="s">
+      <c r="D95" t="s">
         <v>361</v>
-      </c>
-      <c r="C95" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="D95" t="s">
-        <v>363</v>
       </c>
       <c r="E95">
         <v>1</v>
@@ -3452,16 +3454,16 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>362</v>
+      </c>
+      <c r="B96" t="s">
+        <v>363</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>364</v>
       </c>
-      <c r="B96" t="s">
+      <c r="D96" t="s">
         <v>365</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="D96" t="s">
-        <v>367</v>
       </c>
       <c r="E96">
         <v>2</v>
@@ -3472,16 +3474,16 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>366</v>
+      </c>
+      <c r="B97" t="s">
+        <v>367</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="B97" t="s">
+      <c r="D97" t="s">
         <v>369</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>370</v>
-      </c>
-      <c r="D97" t="s">
-        <v>371</v>
       </c>
       <c r="E97">
         <v>19</v>
@@ -3492,16 +3494,16 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>370</v>
+      </c>
+      <c r="B98" t="s">
+        <v>371</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="B98" t="s">
+      <c r="D98" t="s">
         <v>373</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="D98" t="s">
-        <v>375</v>
       </c>
       <c r="E98">
         <v>16</v>
@@ -3512,16 +3514,16 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>374</v>
+      </c>
+      <c r="B99" t="s">
+        <v>375</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="B99" t="s">
+      <c r="D99" t="s">
         <v>377</v>
-      </c>
-      <c r="C99" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="D99" t="s">
-        <v>379</v>
       </c>
       <c r="E99">
         <v>1</v>
@@ -3532,16 +3534,16 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>378</v>
+      </c>
+      <c r="B100" t="s">
+        <v>379</v>
+      </c>
+      <c r="C100" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B100" t="s">
+      <c r="D100" t="s">
         <v>381</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="D100" t="s">
-        <v>383</v>
       </c>
       <c r="E100">
         <v>8</v>
@@ -3552,13 +3554,13 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>382</v>
+      </c>
+      <c r="B101" t="s">
+        <v>383</v>
+      </c>
+      <c r="C101" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="B101" t="s">
-        <v>385</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="D101" t="s">
         <v>15</v>
@@ -3580,7 +3582,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D48153-1644-422E-BF6C-88BBA322D82D}">
   <dimension ref="A3:F103"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3598,10 +3602,10 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3646,7 +3650,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>387</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -3706,7 +3710,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>388</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -4206,16 +4210,13 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>389</v>
+      </c>
+      <c r="C34" t="s">
         <v>124</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>125</v>
-      </c>
-      <c r="C34" t="s">
-        <v>126</v>
-      </c>
-      <c r="D34" t="s">
-        <v>127</v>
       </c>
       <c r="E34">
         <v>10</v>
@@ -4226,16 +4227,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" t="s">
+        <v>127</v>
+      </c>
+      <c r="C35" t="s">
         <v>128</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>129</v>
-      </c>
-      <c r="C35" t="s">
-        <v>130</v>
-      </c>
-      <c r="D35" t="s">
-        <v>131</v>
       </c>
       <c r="E35">
         <v>4</v>
@@ -4246,16 +4247,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" t="s">
         <v>132</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>133</v>
-      </c>
-      <c r="C36" t="s">
-        <v>134</v>
-      </c>
-      <c r="D36" t="s">
-        <v>135</v>
       </c>
       <c r="E36">
         <v>11</v>
@@ -4266,13 +4267,13 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" t="s">
+        <v>135</v>
+      </c>
+      <c r="C37" t="s">
         <v>136</v>
-      </c>
-      <c r="B37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C37" t="s">
-        <v>138</v>
       </c>
       <c r="D37" t="s">
         <v>15</v>
@@ -4286,16 +4287,16 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>137</v>
+      </c>
+      <c r="B38" t="s">
+        <v>138</v>
+      </c>
+      <c r="C38" t="s">
         <v>139</v>
       </c>
-      <c r="B38" t="s">
+      <c r="D38" t="s">
         <v>140</v>
-      </c>
-      <c r="C38" t="s">
-        <v>141</v>
-      </c>
-      <c r="D38" t="s">
-        <v>142</v>
       </c>
       <c r="E38">
         <v>13</v>
@@ -4306,16 +4307,16 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" t="s">
         <v>143</v>
       </c>
-      <c r="B39" t="s">
+      <c r="D39" t="s">
         <v>144</v>
-      </c>
-      <c r="C39" t="s">
-        <v>145</v>
-      </c>
-      <c r="D39" t="s">
-        <v>146</v>
       </c>
       <c r="E39">
         <v>6</v>
@@ -4326,16 +4327,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" t="s">
+        <v>146</v>
+      </c>
+      <c r="C40" t="s">
         <v>147</v>
       </c>
-      <c r="B40" t="s">
+      <c r="D40" t="s">
         <v>148</v>
-      </c>
-      <c r="C40" t="s">
-        <v>149</v>
-      </c>
-      <c r="D40" t="s">
-        <v>150</v>
       </c>
       <c r="E40">
         <v>5</v>
@@ -4346,16 +4347,16 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" t="s">
+        <v>150</v>
+      </c>
+      <c r="C41" t="s">
         <v>151</v>
       </c>
-      <c r="B41" t="s">
+      <c r="D41" t="s">
         <v>152</v>
-      </c>
-      <c r="C41" t="s">
-        <v>153</v>
-      </c>
-      <c r="D41" t="s">
-        <v>154</v>
       </c>
       <c r="E41">
         <v>17</v>
@@ -4366,13 +4367,13 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" t="s">
+        <v>154</v>
+      </c>
+      <c r="C42" t="s">
         <v>155</v>
-      </c>
-      <c r="B42" t="s">
-        <v>156</v>
-      </c>
-      <c r="C42" t="s">
-        <v>157</v>
       </c>
       <c r="D42" t="s">
         <v>39</v>
@@ -4386,16 +4387,16 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" t="s">
         <v>158</v>
       </c>
-      <c r="B43" t="s">
+      <c r="D43" t="s">
         <v>159</v>
-      </c>
-      <c r="C43" t="s">
-        <v>160</v>
-      </c>
-      <c r="D43" t="s">
-        <v>161</v>
       </c>
       <c r="E43">
         <v>16</v>
@@ -4406,16 +4407,16 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B44" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" t="s">
+        <v>161</v>
+      </c>
+      <c r="D44" t="s">
         <v>162</v>
-      </c>
-      <c r="C44" t="s">
-        <v>163</v>
-      </c>
-      <c r="D44" t="s">
-        <v>164</v>
       </c>
       <c r="E44">
         <v>2</v>
@@ -4426,16 +4427,16 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C45" t="s">
         <v>165</v>
       </c>
-      <c r="B45" t="s">
+      <c r="D45" t="s">
         <v>166</v>
-      </c>
-      <c r="C45" t="s">
-        <v>167</v>
-      </c>
-      <c r="D45" t="s">
-        <v>168</v>
       </c>
       <c r="E45">
         <v>4</v>
@@ -4446,16 +4447,16 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>167</v>
+      </c>
+      <c r="B46" t="s">
+        <v>168</v>
+      </c>
+      <c r="C46" t="s">
         <v>169</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>170</v>
-      </c>
-      <c r="C46" t="s">
-        <v>171</v>
-      </c>
-      <c r="D46" t="s">
-        <v>172</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -4466,16 +4467,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>171</v>
+      </c>
+      <c r="B47" t="s">
+        <v>172</v>
+      </c>
+      <c r="C47" t="s">
         <v>173</v>
       </c>
-      <c r="B47" t="s">
+      <c r="D47" t="s">
         <v>174</v>
-      </c>
-      <c r="C47" t="s">
-        <v>175</v>
-      </c>
-      <c r="D47" t="s">
-        <v>176</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -4486,16 +4487,16 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>175</v>
+      </c>
+      <c r="B48" t="s">
+        <v>176</v>
+      </c>
+      <c r="C48" t="s">
         <v>177</v>
       </c>
-      <c r="B48" t="s">
+      <c r="D48" t="s">
         <v>178</v>
-      </c>
-      <c r="C48" t="s">
-        <v>179</v>
-      </c>
-      <c r="D48" t="s">
-        <v>180</v>
       </c>
       <c r="E48">
         <v>6</v>
@@ -4506,16 +4507,16 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>179</v>
+      </c>
+      <c r="B49" t="s">
+        <v>180</v>
+      </c>
+      <c r="C49" t="s">
         <v>181</v>
       </c>
-      <c r="B49" t="s">
-        <v>182</v>
-      </c>
-      <c r="C49" t="s">
-        <v>183</v>
-      </c>
       <c r="D49" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E49">
         <v>20</v>
@@ -4526,16 +4527,16 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>182</v>
+      </c>
+      <c r="B50" t="s">
+        <v>183</v>
+      </c>
+      <c r="C50" t="s">
         <v>184</v>
       </c>
-      <c r="B50" t="s">
+      <c r="D50" t="s">
         <v>185</v>
-      </c>
-      <c r="C50" t="s">
-        <v>186</v>
-      </c>
-      <c r="D50" t="s">
-        <v>187</v>
       </c>
       <c r="E50">
         <v>1</v>
@@ -4546,16 +4547,16 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>186</v>
+      </c>
+      <c r="B51" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" t="s">
         <v>188</v>
       </c>
-      <c r="B51" t="s">
+      <c r="D51" t="s">
         <v>189</v>
-      </c>
-      <c r="C51" t="s">
-        <v>190</v>
-      </c>
-      <c r="D51" t="s">
-        <v>191</v>
       </c>
       <c r="E51">
         <v>19</v>
@@ -4566,16 +4567,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>190</v>
+      </c>
+      <c r="B52" t="s">
+        <v>191</v>
+      </c>
+      <c r="C52" t="s">
         <v>192</v>
       </c>
-      <c r="B52" t="s">
+      <c r="D52" t="s">
         <v>193</v>
-      </c>
-      <c r="C52" t="s">
-        <v>194</v>
-      </c>
-      <c r="D52" t="s">
-        <v>195</v>
       </c>
       <c r="E52">
         <v>2</v>
@@ -4586,16 +4587,16 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>194</v>
+      </c>
+      <c r="B53" t="s">
+        <v>195</v>
+      </c>
+      <c r="C53" t="s">
         <v>196</v>
       </c>
-      <c r="B53" t="s">
+      <c r="D53" t="s">
         <v>197</v>
-      </c>
-      <c r="C53" t="s">
-        <v>198</v>
-      </c>
-      <c r="D53" t="s">
-        <v>199</v>
       </c>
       <c r="E53">
         <v>15</v>
@@ -4606,16 +4607,16 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>198</v>
+      </c>
+      <c r="B54" t="s">
+        <v>199</v>
+      </c>
+      <c r="C54" t="s">
         <v>200</v>
       </c>
-      <c r="B54" t="s">
+      <c r="D54" t="s">
         <v>201</v>
-      </c>
-      <c r="C54" t="s">
-        <v>202</v>
-      </c>
-      <c r="D54" t="s">
-        <v>203</v>
       </c>
       <c r="E54">
         <v>20</v>
@@ -4626,16 +4627,16 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>202</v>
+      </c>
+      <c r="B55" t="s">
+        <v>203</v>
+      </c>
+      <c r="C55" t="s">
         <v>204</v>
       </c>
-      <c r="B55" t="s">
+      <c r="D55" t="s">
         <v>205</v>
-      </c>
-      <c r="C55" t="s">
-        <v>206</v>
-      </c>
-      <c r="D55" t="s">
-        <v>207</v>
       </c>
       <c r="E55">
         <v>10</v>
@@ -4646,16 +4647,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>206</v>
+      </c>
+      <c r="B56" t="s">
+        <v>207</v>
+      </c>
+      <c r="C56" t="s">
         <v>208</v>
       </c>
-      <c r="B56" t="s">
+      <c r="D56" t="s">
         <v>209</v>
-      </c>
-      <c r="C56" t="s">
-        <v>210</v>
-      </c>
-      <c r="D56" t="s">
-        <v>211</v>
       </c>
       <c r="E56">
         <v>17</v>
@@ -4666,16 +4667,16 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>210</v>
+      </c>
+      <c r="B57" t="s">
+        <v>211</v>
+      </c>
+      <c r="C57" t="s">
         <v>212</v>
       </c>
-      <c r="B57" t="s">
+      <c r="D57" t="s">
         <v>213</v>
-      </c>
-      <c r="C57" t="s">
-        <v>214</v>
-      </c>
-      <c r="D57" t="s">
-        <v>215</v>
       </c>
       <c r="E57">
         <v>2</v>
@@ -4686,16 +4687,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>214</v>
+      </c>
+      <c r="B58" t="s">
+        <v>215</v>
+      </c>
+      <c r="C58" t="s">
         <v>216</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
         <v>217</v>
-      </c>
-      <c r="C58" t="s">
-        <v>218</v>
-      </c>
-      <c r="D58" t="s">
-        <v>219</v>
       </c>
       <c r="E58">
         <v>11</v>
@@ -4706,16 +4707,16 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>218</v>
+      </c>
+      <c r="B59" t="s">
+        <v>219</v>
+      </c>
+      <c r="C59" t="s">
         <v>220</v>
       </c>
-      <c r="B59" t="s">
+      <c r="D59" t="s">
         <v>221</v>
-      </c>
-      <c r="C59" t="s">
-        <v>222</v>
-      </c>
-      <c r="D59" t="s">
-        <v>223</v>
       </c>
       <c r="E59">
         <v>13</v>
@@ -4726,16 +4727,16 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>222</v>
+      </c>
+      <c r="B60" t="s">
+        <v>223</v>
+      </c>
+      <c r="C60" t="s">
         <v>224</v>
       </c>
-      <c r="B60" t="s">
-        <v>225</v>
-      </c>
-      <c r="C60" t="s">
-        <v>226</v>
-      </c>
       <c r="D60" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E60">
         <v>1</v>
@@ -4746,16 +4747,16 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>225</v>
+      </c>
+      <c r="B61" t="s">
+        <v>226</v>
+      </c>
+      <c r="C61" t="s">
         <v>227</v>
       </c>
-      <c r="B61" t="s">
+      <c r="D61" t="s">
         <v>228</v>
-      </c>
-      <c r="C61" t="s">
-        <v>229</v>
-      </c>
-      <c r="D61" t="s">
-        <v>230</v>
       </c>
       <c r="E61">
         <v>9</v>
@@ -4766,16 +4767,16 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>229</v>
+      </c>
+      <c r="B62" t="s">
+        <v>230</v>
+      </c>
+      <c r="C62" t="s">
         <v>231</v>
       </c>
-      <c r="B62" t="s">
+      <c r="D62" t="s">
         <v>232</v>
-      </c>
-      <c r="C62" t="s">
-        <v>233</v>
-      </c>
-      <c r="D62" t="s">
-        <v>234</v>
       </c>
       <c r="E62">
         <v>1</v>
@@ -4786,16 +4787,16 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>233</v>
+      </c>
+      <c r="B63" t="s">
+        <v>234</v>
+      </c>
+      <c r="C63" t="s">
         <v>235</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" t="s">
         <v>236</v>
-      </c>
-      <c r="C63" t="s">
-        <v>237</v>
-      </c>
-      <c r="D63" t="s">
-        <v>238</v>
       </c>
       <c r="E63">
         <v>3</v>
@@ -4806,13 +4807,13 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>237</v>
+      </c>
+      <c r="B64" t="s">
+        <v>238</v>
+      </c>
+      <c r="C64" t="s">
         <v>239</v>
-      </c>
-      <c r="B64" t="s">
-        <v>240</v>
-      </c>
-      <c r="C64" t="s">
-        <v>241</v>
       </c>
       <c r="D64" t="s">
         <v>95</v>
@@ -4826,16 +4827,16 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>240</v>
+      </c>
+      <c r="B65" t="s">
+        <v>241</v>
+      </c>
+      <c r="C65" t="s">
         <v>242</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" t="s">
         <v>243</v>
-      </c>
-      <c r="C65" t="s">
-        <v>244</v>
-      </c>
-      <c r="D65" t="s">
-        <v>245</v>
       </c>
       <c r="E65">
         <v>8</v>
@@ -4846,16 +4847,16 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>244</v>
+      </c>
+      <c r="B66" t="s">
+        <v>245</v>
+      </c>
+      <c r="C66" t="s">
         <v>246</v>
       </c>
-      <c r="B66" t="s">
+      <c r="D66" t="s">
         <v>247</v>
-      </c>
-      <c r="C66" t="s">
-        <v>248</v>
-      </c>
-      <c r="D66" t="s">
-        <v>249</v>
       </c>
       <c r="E66">
         <v>7</v>
@@ -4866,16 +4867,16 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>248</v>
+      </c>
+      <c r="B67" t="s">
+        <v>249</v>
+      </c>
+      <c r="C67" t="s">
         <v>250</v>
       </c>
-      <c r="B67" t="s">
+      <c r="D67" t="s">
         <v>251</v>
-      </c>
-      <c r="C67" t="s">
-        <v>252</v>
-      </c>
-      <c r="D67" t="s">
-        <v>253</v>
       </c>
       <c r="E67">
         <v>1</v>
@@ -4886,16 +4887,16 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>252</v>
+      </c>
+      <c r="B68" t="s">
+        <v>253</v>
+      </c>
+      <c r="C68" t="s">
         <v>254</v>
       </c>
-      <c r="B68" t="s">
-        <v>255</v>
-      </c>
-      <c r="C68" t="s">
-        <v>256</v>
-      </c>
       <c r="D68" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E68">
         <v>7</v>
@@ -4906,16 +4907,16 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>255</v>
+      </c>
+      <c r="B69" t="s">
+        <v>256</v>
+      </c>
+      <c r="C69" t="s">
         <v>257</v>
       </c>
-      <c r="B69" t="s">
+      <c r="D69" t="s">
         <v>258</v>
-      </c>
-      <c r="C69" t="s">
-        <v>259</v>
-      </c>
-      <c r="D69" t="s">
-        <v>260</v>
       </c>
       <c r="E69">
         <v>17</v>
@@ -4926,16 +4927,16 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>259</v>
+      </c>
+      <c r="B70" t="s">
+        <v>260</v>
+      </c>
+      <c r="C70" t="s">
         <v>261</v>
       </c>
-      <c r="B70" t="s">
+      <c r="D70" t="s">
         <v>262</v>
-      </c>
-      <c r="C70" t="s">
-        <v>263</v>
-      </c>
-      <c r="D70" t="s">
-        <v>264</v>
       </c>
       <c r="E70">
         <v>6</v>
@@ -4946,16 +4947,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>263</v>
+      </c>
+      <c r="B71" t="s">
+        <v>264</v>
+      </c>
+      <c r="C71" t="s">
         <v>265</v>
       </c>
-      <c r="B71" t="s">
-        <v>266</v>
-      </c>
-      <c r="C71" t="s">
-        <v>267</v>
-      </c>
       <c r="D71" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E71">
         <v>20</v>
@@ -4966,16 +4967,16 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>266</v>
+      </c>
+      <c r="B72" t="s">
+        <v>267</v>
+      </c>
+      <c r="C72" t="s">
         <v>268</v>
       </c>
-      <c r="B72" t="s">
+      <c r="D72" t="s">
         <v>269</v>
-      </c>
-      <c r="C72" t="s">
-        <v>270</v>
-      </c>
-      <c r="D72" t="s">
-        <v>271</v>
       </c>
       <c r="E72">
         <v>11</v>
@@ -4986,16 +4987,16 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>270</v>
+      </c>
+      <c r="B73" t="s">
+        <v>271</v>
+      </c>
+      <c r="C73" t="s">
         <v>272</v>
       </c>
-      <c r="B73" t="s">
+      <c r="D73" t="s">
         <v>273</v>
-      </c>
-      <c r="C73" t="s">
-        <v>274</v>
-      </c>
-      <c r="D73" t="s">
-        <v>275</v>
       </c>
       <c r="E73">
         <v>1</v>
@@ -5009,13 +5010,13 @@
         <v>40</v>
       </c>
       <c r="B74" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C74" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D74" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="E74">
         <v>13</v>
@@ -5026,16 +5027,16 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>276</v>
+      </c>
+      <c r="B75" t="s">
+        <v>277</v>
+      </c>
+      <c r="C75" t="s">
         <v>278</v>
       </c>
-      <c r="B75" t="s">
+      <c r="D75" t="s">
         <v>279</v>
-      </c>
-      <c r="C75" t="s">
-        <v>280</v>
-      </c>
-      <c r="D75" t="s">
-        <v>281</v>
       </c>
       <c r="E75">
         <v>16</v>
@@ -5046,16 +5047,16 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>280</v>
+      </c>
+      <c r="B76" t="s">
+        <v>281</v>
+      </c>
+      <c r="C76" t="s">
         <v>282</v>
       </c>
-      <c r="B76" t="s">
+      <c r="D76" t="s">
         <v>283</v>
-      </c>
-      <c r="C76" t="s">
-        <v>284</v>
-      </c>
-      <c r="D76" t="s">
-        <v>285</v>
       </c>
       <c r="E76">
         <v>10</v>
@@ -5066,16 +5067,16 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
+        <v>284</v>
+      </c>
+      <c r="B77" t="s">
+        <v>285</v>
+      </c>
+      <c r="C77" t="s">
         <v>286</v>
       </c>
-      <c r="B77" t="s">
-        <v>287</v>
-      </c>
-      <c r="C77" t="s">
-        <v>288</v>
-      </c>
       <c r="D77" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E77">
         <v>13</v>
@@ -5086,16 +5087,16 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>287</v>
+      </c>
+      <c r="B78" t="s">
+        <v>288</v>
+      </c>
+      <c r="C78" t="s">
         <v>289</v>
       </c>
-      <c r="B78" t="s">
+      <c r="D78" t="s">
         <v>290</v>
-      </c>
-      <c r="C78" t="s">
-        <v>291</v>
-      </c>
-      <c r="D78" t="s">
-        <v>292</v>
       </c>
       <c r="E78">
         <v>8</v>
@@ -5106,16 +5107,16 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>291</v>
+      </c>
+      <c r="B79" t="s">
+        <v>292</v>
+      </c>
+      <c r="C79" t="s">
         <v>293</v>
       </c>
-      <c r="B79" t="s">
+      <c r="D79" t="s">
         <v>294</v>
-      </c>
-      <c r="C79" t="s">
-        <v>295</v>
-      </c>
-      <c r="D79" t="s">
-        <v>296</v>
       </c>
       <c r="E79">
         <v>7</v>
@@ -5126,13 +5127,13 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>295</v>
+      </c>
+      <c r="B80" t="s">
+        <v>296</v>
+      </c>
+      <c r="C80" t="s">
         <v>297</v>
-      </c>
-      <c r="B80" t="s">
-        <v>298</v>
-      </c>
-      <c r="C80" t="s">
-        <v>299</v>
       </c>
       <c r="D80" t="s">
         <v>67</v>
@@ -5146,16 +5147,16 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
+        <v>298</v>
+      </c>
+      <c r="B81" t="s">
+        <v>299</v>
+      </c>
+      <c r="C81" t="s">
         <v>300</v>
       </c>
-      <c r="B81" t="s">
+      <c r="D81" t="s">
         <v>301</v>
-      </c>
-      <c r="C81" t="s">
-        <v>302</v>
-      </c>
-      <c r="D81" t="s">
-        <v>303</v>
       </c>
       <c r="E81">
         <v>13</v>
@@ -5166,16 +5167,16 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>302</v>
+      </c>
+      <c r="B82" t="s">
+        <v>303</v>
+      </c>
+      <c r="C82" t="s">
         <v>304</v>
       </c>
-      <c r="B82" t="s">
+      <c r="D82" t="s">
         <v>305</v>
-      </c>
-      <c r="C82" t="s">
-        <v>306</v>
-      </c>
-      <c r="D82" t="s">
-        <v>307</v>
       </c>
       <c r="E82">
         <v>17</v>
@@ -5186,16 +5187,16 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>306</v>
+      </c>
+      <c r="B83" t="s">
+        <v>307</v>
+      </c>
+      <c r="C83" t="s">
         <v>308</v>
       </c>
-      <c r="B83" t="s">
+      <c r="D83" t="s">
         <v>309</v>
-      </c>
-      <c r="C83" t="s">
-        <v>310</v>
-      </c>
-      <c r="D83" t="s">
-        <v>311</v>
       </c>
       <c r="E83">
         <v>12</v>
@@ -5206,13 +5207,13 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>310</v>
+      </c>
+      <c r="B84" t="s">
+        <v>311</v>
+      </c>
+      <c r="C84" t="s">
         <v>312</v>
-      </c>
-      <c r="B84" t="s">
-        <v>313</v>
-      </c>
-      <c r="C84" t="s">
-        <v>314</v>
       </c>
       <c r="D84" t="s">
         <v>27</v>
@@ -5226,16 +5227,16 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>313</v>
+      </c>
+      <c r="B85" t="s">
+        <v>314</v>
+      </c>
+      <c r="C85" t="s">
         <v>315</v>
       </c>
-      <c r="B85" t="s">
+      <c r="D85" t="s">
         <v>316</v>
-      </c>
-      <c r="C85" t="s">
-        <v>317</v>
-      </c>
-      <c r="D85" t="s">
-        <v>318</v>
       </c>
       <c r="E85">
         <v>15</v>
@@ -5246,16 +5247,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
+        <v>317</v>
+      </c>
+      <c r="B86" t="s">
+        <v>318</v>
+      </c>
+      <c r="C86" t="s">
         <v>319</v>
       </c>
-      <c r="B86" t="s">
+      <c r="D86" t="s">
         <v>320</v>
-      </c>
-      <c r="C86" t="s">
-        <v>321</v>
-      </c>
-      <c r="D86" t="s">
-        <v>322</v>
       </c>
       <c r="E86">
         <v>19</v>
@@ -5266,16 +5267,16 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
+        <v>321</v>
+      </c>
+      <c r="B87" t="s">
+        <v>322</v>
+      </c>
+      <c r="C87" t="s">
         <v>323</v>
       </c>
-      <c r="B87" t="s">
+      <c r="D87" t="s">
         <v>324</v>
-      </c>
-      <c r="C87" t="s">
-        <v>325</v>
-      </c>
-      <c r="D87" t="s">
-        <v>326</v>
       </c>
       <c r="E87">
         <v>12</v>
@@ -5286,16 +5287,16 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
+        <v>325</v>
+      </c>
+      <c r="B88" t="s">
+        <v>326</v>
+      </c>
+      <c r="C88" t="s">
         <v>327</v>
       </c>
-      <c r="B88" t="s">
+      <c r="D88" t="s">
         <v>328</v>
-      </c>
-      <c r="C88" t="s">
-        <v>329</v>
-      </c>
-      <c r="D88" t="s">
-        <v>330</v>
       </c>
       <c r="E88">
         <v>14</v>
@@ -5306,16 +5307,16 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
+        <v>329</v>
+      </c>
+      <c r="B89" t="s">
+        <v>330</v>
+      </c>
+      <c r="C89" t="s">
         <v>331</v>
       </c>
-      <c r="B89" t="s">
+      <c r="D89" t="s">
         <v>332</v>
-      </c>
-      <c r="C89" t="s">
-        <v>333</v>
-      </c>
-      <c r="D89" t="s">
-        <v>334</v>
       </c>
       <c r="E89">
         <v>3</v>
@@ -5326,16 +5327,16 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
+        <v>333</v>
+      </c>
+      <c r="B90" t="s">
+        <v>334</v>
+      </c>
+      <c r="C90" t="s">
         <v>335</v>
       </c>
-      <c r="B90" t="s">
+      <c r="D90" t="s">
         <v>336</v>
-      </c>
-      <c r="C90" t="s">
-        <v>337</v>
-      </c>
-      <c r="D90" t="s">
-        <v>338</v>
       </c>
       <c r="E90">
         <v>2</v>
@@ -5346,16 +5347,16 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
+        <v>337</v>
+      </c>
+      <c r="B91" t="s">
+        <v>338</v>
+      </c>
+      <c r="C91" t="s">
         <v>339</v>
       </c>
-      <c r="B91" t="s">
+      <c r="D91" t="s">
         <v>340</v>
-      </c>
-      <c r="C91" t="s">
-        <v>341</v>
-      </c>
-      <c r="D91" t="s">
-        <v>342</v>
       </c>
       <c r="E91">
         <v>2</v>
@@ -5366,13 +5367,13 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>341</v>
+      </c>
+      <c r="B92" t="s">
+        <v>342</v>
+      </c>
+      <c r="C92" t="s">
         <v>343</v>
-      </c>
-      <c r="B92" t="s">
-        <v>344</v>
-      </c>
-      <c r="C92" t="s">
-        <v>345</v>
       </c>
       <c r="D92" t="s">
         <v>123</v>
@@ -5386,16 +5387,16 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>344</v>
+      </c>
+      <c r="B93" t="s">
+        <v>345</v>
+      </c>
+      <c r="C93" t="s">
         <v>346</v>
       </c>
-      <c r="B93" t="s">
-        <v>347</v>
-      </c>
-      <c r="C93" t="s">
-        <v>348</v>
-      </c>
       <c r="D93" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E93">
         <v>19</v>
@@ -5406,16 +5407,16 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
+        <v>347</v>
+      </c>
+      <c r="B94" t="s">
+        <v>348</v>
+      </c>
+      <c r="C94" t="s">
         <v>349</v>
       </c>
-      <c r="B94" t="s">
+      <c r="D94" t="s">
         <v>350</v>
-      </c>
-      <c r="C94" t="s">
-        <v>351</v>
-      </c>
-      <c r="D94" t="s">
-        <v>352</v>
       </c>
       <c r="E94">
         <v>9</v>
@@ -5426,16 +5427,16 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>351</v>
+      </c>
+      <c r="B95" t="s">
+        <v>352</v>
+      </c>
+      <c r="C95" t="s">
         <v>353</v>
       </c>
-      <c r="B95" t="s">
-        <v>354</v>
-      </c>
-      <c r="C95" t="s">
-        <v>355</v>
-      </c>
       <c r="D95" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E95">
         <v>10</v>
@@ -5446,16 +5447,16 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>354</v>
+      </c>
+      <c r="B96" t="s">
+        <v>355</v>
+      </c>
+      <c r="C96" t="s">
         <v>356</v>
       </c>
-      <c r="B96" t="s">
+      <c r="D96" t="s">
         <v>357</v>
-      </c>
-      <c r="C96" t="s">
-        <v>358</v>
-      </c>
-      <c r="D96" t="s">
-        <v>359</v>
       </c>
       <c r="E96">
         <v>1</v>
@@ -5466,16 +5467,16 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
+        <v>358</v>
+      </c>
+      <c r="B97" t="s">
+        <v>359</v>
+      </c>
+      <c r="C97" t="s">
         <v>360</v>
       </c>
-      <c r="B97" t="s">
+      <c r="D97" t="s">
         <v>361</v>
-      </c>
-      <c r="C97" t="s">
-        <v>362</v>
-      </c>
-      <c r="D97" t="s">
-        <v>363</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -5486,16 +5487,16 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
+        <v>362</v>
+      </c>
+      <c r="B98" t="s">
+        <v>363</v>
+      </c>
+      <c r="C98" t="s">
         <v>364</v>
       </c>
-      <c r="B98" t="s">
+      <c r="D98" t="s">
         <v>365</v>
-      </c>
-      <c r="C98" t="s">
-        <v>366</v>
-      </c>
-      <c r="D98" t="s">
-        <v>367</v>
       </c>
       <c r="E98">
         <v>2</v>
@@ -5506,16 +5507,16 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>366</v>
+      </c>
+      <c r="B99" t="s">
+        <v>367</v>
+      </c>
+      <c r="C99" t="s">
         <v>368</v>
       </c>
-      <c r="B99" t="s">
+      <c r="D99" t="s">
         <v>369</v>
-      </c>
-      <c r="C99" t="s">
-        <v>370</v>
-      </c>
-      <c r="D99" t="s">
-        <v>371</v>
       </c>
       <c r="E99">
         <v>19</v>
@@ -5526,16 +5527,16 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
+        <v>370</v>
+      </c>
+      <c r="B100" t="s">
+        <v>371</v>
+      </c>
+      <c r="C100" t="s">
         <v>372</v>
       </c>
-      <c r="B100" t="s">
+      <c r="D100" t="s">
         <v>373</v>
-      </c>
-      <c r="C100" t="s">
-        <v>374</v>
-      </c>
-      <c r="D100" t="s">
-        <v>375</v>
       </c>
       <c r="E100">
         <v>16</v>
@@ -5546,16 +5547,16 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
+        <v>374</v>
+      </c>
+      <c r="B101" t="s">
+        <v>375</v>
+      </c>
+      <c r="C101" t="s">
         <v>376</v>
       </c>
-      <c r="B101" t="s">
+      <c r="D101" t="s">
         <v>377</v>
-      </c>
-      <c r="C101" t="s">
-        <v>378</v>
-      </c>
-      <c r="D101" t="s">
-        <v>379</v>
       </c>
       <c r="E101">
         <v>1</v>
@@ -5566,16 +5567,16 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
+        <v>378</v>
+      </c>
+      <c r="B102" t="s">
+        <v>379</v>
+      </c>
+      <c r="C102" t="s">
         <v>380</v>
       </c>
-      <c r="B102" t="s">
+      <c r="D102" t="s">
         <v>381</v>
-      </c>
-      <c r="C102" t="s">
-        <v>382</v>
-      </c>
-      <c r="D102" t="s">
-        <v>383</v>
       </c>
       <c r="E102">
         <v>8</v>
@@ -5586,13 +5587,13 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>382</v>
+      </c>
+      <c r="B103" t="s">
+        <v>383</v>
+      </c>
+      <c r="C103" t="s">
         <v>384</v>
-      </c>
-      <c r="B103" t="s">
-        <v>385</v>
-      </c>
-      <c r="C103" t="s">
-        <v>386</v>
       </c>
       <c r="D103" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
- Fixed cellRange issue and updated test case
Signed-off-by: LeandroC89 <leandroadao3@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/krangl/data/ExcelReadExample.xlsx
+++ b/src/test/resources/krangl/data/ExcelReadExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LCouto\IdeaProjects\krangl\src\test\resources\krangl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E90D4C1-E0F3-49AE-8E80-58884565C9AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711EC427-5760-4F92-BEAA-E4D4075BEA04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstSheet" sheetId="1" r:id="rId1"/>
@@ -1543,9 +1543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3580,2028 +3578,2036 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D48153-1644-422E-BF6C-88BBA322D82D}">
-  <dimension ref="A3:F103"/>
+  <dimension ref="E3:J103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="3" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="I3" t="s">
         <v>385</v>
       </c>
-      <c r="F3" t="s">
+      <c r="J3" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="G4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="E4">
+      <c r="I4">
         <v>20</v>
       </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
         <v>11</v>
       </c>
-      <c r="E5">
+      <c r="I5">
         <v>17</v>
       </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
         <v>387</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="G6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="H6" t="s">
         <v>15</v>
       </c>
-      <c r="E6">
+      <c r="I6">
         <v>14</v>
       </c>
-      <c r="F6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="F7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
+      <c r="G7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="H7" t="s">
         <v>19</v>
       </c>
-      <c r="E7">
+      <c r="I7">
         <v>10</v>
       </c>
-      <c r="F7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="F8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="G8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" t="s">
+      <c r="H8" t="s">
         <v>23</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
         <v>388</v>
       </c>
-      <c r="B9" t="s">
+      <c r="F9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
+      <c r="G9" t="s">
         <v>26</v>
       </c>
-      <c r="D9" t="s">
+      <c r="H9" t="s">
         <v>27</v>
       </c>
-      <c r="E9">
+      <c r="I9">
         <v>18</v>
       </c>
-      <c r="F9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
         <v>28</v>
       </c>
-      <c r="B10" t="s">
+      <c r="F10" t="s">
         <v>29</v>
       </c>
-      <c r="C10" t="s">
+      <c r="G10" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="s">
+      <c r="H10" t="s">
         <v>31</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" t="s">
+      <c r="F11" t="s">
         <v>33</v>
       </c>
-      <c r="C11" t="s">
+      <c r="G11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" t="s">
+      <c r="H11" t="s">
         <v>35</v>
       </c>
-      <c r="E11">
+      <c r="I11">
         <v>16</v>
       </c>
-      <c r="F11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
         <v>36</v>
       </c>
-      <c r="B12" t="s">
+      <c r="F12" t="s">
         <v>37</v>
       </c>
-      <c r="C12" t="s">
+      <c r="G12" t="s">
         <v>38</v>
       </c>
-      <c r="D12" t="s">
+      <c r="H12" t="s">
         <v>39</v>
       </c>
-      <c r="E12">
+      <c r="I12">
         <v>4</v>
       </c>
-      <c r="F12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
+      <c r="F13" t="s">
         <v>41</v>
       </c>
-      <c r="C13" t="s">
+      <c r="G13" t="s">
         <v>42</v>
       </c>
-      <c r="D13" t="s">
+      <c r="H13" t="s">
         <v>43</v>
       </c>
-      <c r="E13">
+      <c r="I13">
         <v>7</v>
       </c>
-      <c r="F13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="F14" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
+      <c r="G14" t="s">
         <v>46</v>
       </c>
-      <c r="D14" t="s">
+      <c r="H14" t="s">
         <v>47</v>
       </c>
-      <c r="E14">
+      <c r="I14">
         <v>5</v>
       </c>
-      <c r="F14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
         <v>48</v>
       </c>
-      <c r="B15" t="s">
+      <c r="F15" t="s">
         <v>49</v>
       </c>
-      <c r="C15" t="s">
+      <c r="G15" t="s">
         <v>50</v>
       </c>
-      <c r="D15" t="s">
+      <c r="H15" t="s">
         <v>51</v>
       </c>
-      <c r="E15">
+      <c r="I15">
         <v>2</v>
       </c>
-      <c r="F15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
         <v>52</v>
       </c>
-      <c r="B16" t="s">
+      <c r="F16" t="s">
         <v>53</v>
       </c>
-      <c r="C16" t="s">
+      <c r="G16" t="s">
         <v>54</v>
       </c>
-      <c r="D16" t="s">
+      <c r="H16" t="s">
         <v>55</v>
       </c>
-      <c r="E16">
+      <c r="I16">
         <v>9</v>
       </c>
-      <c r="F16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
         <v>56</v>
       </c>
-      <c r="B17" t="s">
+      <c r="F17" t="s">
         <v>57</v>
       </c>
-      <c r="C17" t="s">
+      <c r="G17" t="s">
         <v>58</v>
       </c>
-      <c r="D17" t="s">
+      <c r="H17" t="s">
         <v>59</v>
       </c>
-      <c r="E17">
+      <c r="I17">
         <v>3</v>
       </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
         <v>60</v>
       </c>
-      <c r="B18" t="s">
+      <c r="F18" t="s">
         <v>61</v>
       </c>
-      <c r="C18" t="s">
+      <c r="G18" t="s">
         <v>62</v>
       </c>
-      <c r="D18" t="s">
+      <c r="H18" t="s">
         <v>63</v>
       </c>
-      <c r="E18">
+      <c r="I18">
         <v>14</v>
       </c>
-      <c r="F18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
         <v>64</v>
       </c>
-      <c r="B19" t="s">
+      <c r="F19" t="s">
         <v>65</v>
       </c>
-      <c r="C19" t="s">
+      <c r="G19" t="s">
         <v>66</v>
       </c>
-      <c r="D19" t="s">
+      <c r="H19" t="s">
         <v>67</v>
       </c>
-      <c r="E19">
+      <c r="I19">
         <v>8</v>
       </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
         <v>68</v>
       </c>
-      <c r="B20" t="s">
+      <c r="F20" t="s">
         <v>69</v>
       </c>
-      <c r="C20" t="s">
+      <c r="G20" t="s">
         <v>70</v>
       </c>
-      <c r="D20" t="s">
+      <c r="H20" t="s">
         <v>71</v>
       </c>
-      <c r="E20">
+      <c r="I20">
         <v>13</v>
       </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
         <v>72</v>
       </c>
-      <c r="B21" t="s">
+      <c r="F21" t="s">
         <v>73</v>
       </c>
-      <c r="C21" t="s">
+      <c r="G21" t="s">
         <v>74</v>
       </c>
-      <c r="D21" t="s">
+      <c r="H21" t="s">
         <v>75</v>
       </c>
-      <c r="E21">
+      <c r="I21">
         <v>7</v>
       </c>
-      <c r="F21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
         <v>76</v>
       </c>
-      <c r="B22" t="s">
+      <c r="F22" t="s">
         <v>77</v>
       </c>
-      <c r="C22" t="s">
+      <c r="G22" t="s">
         <v>78</v>
       </c>
-      <c r="D22" t="s">
+      <c r="H22" t="s">
         <v>79</v>
       </c>
-      <c r="E22">
+      <c r="I22">
         <v>7</v>
       </c>
-      <c r="F22" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
         <v>80</v>
       </c>
-      <c r="B23" t="s">
+      <c r="F23" t="s">
         <v>81</v>
       </c>
-      <c r="C23" t="s">
+      <c r="G23" t="s">
         <v>82</v>
       </c>
-      <c r="D23" t="s">
+      <c r="H23" t="s">
         <v>83</v>
       </c>
-      <c r="E23">
+      <c r="I23">
         <v>8</v>
       </c>
-      <c r="F23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
         <v>84</v>
       </c>
-      <c r="B24" t="s">
+      <c r="F24" t="s">
         <v>85</v>
       </c>
-      <c r="C24" t="s">
+      <c r="G24" t="s">
         <v>86</v>
       </c>
-      <c r="D24" t="s">
+      <c r="H24" t="s">
         <v>87</v>
       </c>
-      <c r="E24">
+      <c r="I24">
         <v>16</v>
       </c>
-      <c r="F24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
         <v>88</v>
       </c>
-      <c r="B25" t="s">
+      <c r="F25" t="s">
         <v>89</v>
       </c>
-      <c r="C25" t="s">
+      <c r="G25" t="s">
         <v>90</v>
       </c>
-      <c r="D25" t="s">
+      <c r="H25" t="s">
         <v>91</v>
       </c>
-      <c r="E25">
+      <c r="I25">
         <v>3</v>
       </c>
-      <c r="F25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
         <v>92</v>
       </c>
-      <c r="B26" t="s">
+      <c r="F26" t="s">
         <v>93</v>
       </c>
-      <c r="C26" t="s">
+      <c r="G26" t="s">
         <v>94</v>
       </c>
-      <c r="D26" t="s">
+      <c r="H26" t="s">
         <v>95</v>
       </c>
-      <c r="E26">
+      <c r="I26">
         <v>13</v>
       </c>
-      <c r="F26" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
         <v>96</v>
       </c>
-      <c r="B27" t="s">
+      <c r="F27" t="s">
         <v>97</v>
       </c>
-      <c r="C27" t="s">
+      <c r="G27" t="s">
         <v>98</v>
       </c>
-      <c r="D27" t="s">
+      <c r="H27" t="s">
         <v>99</v>
       </c>
-      <c r="E27">
+      <c r="I27">
         <v>20</v>
       </c>
-      <c r="F27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="J27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
         <v>100</v>
       </c>
-      <c r="B28" t="s">
+      <c r="F28" t="s">
         <v>101</v>
       </c>
-      <c r="C28" t="s">
+      <c r="G28" t="s">
         <v>102</v>
       </c>
-      <c r="D28" t="s">
+      <c r="H28" t="s">
         <v>103</v>
       </c>
-      <c r="E28">
+      <c r="I28">
         <v>7</v>
       </c>
-      <c r="F28" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
         <v>104</v>
       </c>
-      <c r="B29" t="s">
+      <c r="F29" t="s">
         <v>105</v>
       </c>
-      <c r="C29" t="s">
+      <c r="G29" t="s">
         <v>106</v>
       </c>
-      <c r="D29" t="s">
+      <c r="H29" t="s">
         <v>107</v>
       </c>
-      <c r="E29">
+      <c r="I29">
         <v>12</v>
       </c>
-      <c r="F29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="J29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
         <v>108</v>
       </c>
-      <c r="B30" t="s">
+      <c r="F30" t="s">
         <v>109</v>
       </c>
-      <c r="C30" t="s">
+      <c r="G30" t="s">
         <v>110</v>
       </c>
-      <c r="D30" t="s">
+      <c r="H30" t="s">
         <v>111</v>
       </c>
-      <c r="E30">
+      <c r="I30">
         <v>4</v>
       </c>
-      <c r="F30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
         <v>112</v>
       </c>
-      <c r="B31" t="s">
+      <c r="F31" t="s">
         <v>113</v>
       </c>
-      <c r="C31" t="s">
+      <c r="G31" t="s">
         <v>114</v>
       </c>
-      <c r="D31" t="s">
+      <c r="H31" t="s">
         <v>115</v>
       </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="F31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
         <v>116</v>
       </c>
-      <c r="B32" t="s">
+      <c r="F32" t="s">
         <v>117</v>
       </c>
-      <c r="C32" t="s">
+      <c r="G32" t="s">
         <v>118</v>
       </c>
-      <c r="D32" t="s">
+      <c r="H32" t="s">
         <v>119</v>
       </c>
-      <c r="E32">
+      <c r="I32">
         <v>7</v>
       </c>
-      <c r="F32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
         <v>120</v>
       </c>
-      <c r="B33" t="s">
+      <c r="F33" t="s">
         <v>121</v>
       </c>
-      <c r="C33" t="s">
+      <c r="G33" t="s">
         <v>122</v>
       </c>
-      <c r="D33" t="s">
+      <c r="H33" t="s">
         <v>123</v>
       </c>
-      <c r="E33">
+      <c r="I33">
         <v>14</v>
       </c>
-      <c r="F33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
         <v>389</v>
       </c>
-      <c r="C34" t="s">
+      <c r="G34" t="s">
         <v>124</v>
       </c>
-      <c r="D34" t="s">
+      <c r="H34" t="s">
         <v>125</v>
       </c>
-      <c r="E34">
+      <c r="I34">
         <v>10</v>
       </c>
-      <c r="F34" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
         <v>126</v>
       </c>
-      <c r="B35" t="s">
+      <c r="F35" t="s">
         <v>127</v>
       </c>
-      <c r="C35" t="s">
+      <c r="G35" t="s">
         <v>128</v>
       </c>
-      <c r="D35" t="s">
+      <c r="H35" t="s">
         <v>129</v>
       </c>
-      <c r="E35">
+      <c r="I35">
         <v>4</v>
       </c>
-      <c r="F35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
         <v>130</v>
       </c>
-      <c r="B36" t="s">
+      <c r="F36" t="s">
         <v>131</v>
       </c>
-      <c r="C36" t="s">
+      <c r="G36" t="s">
         <v>132</v>
       </c>
-      <c r="D36" t="s">
+      <c r="H36" t="s">
         <v>133</v>
       </c>
-      <c r="E36">
+      <c r="I36">
         <v>11</v>
       </c>
-      <c r="F36" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="J36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
         <v>134</v>
       </c>
-      <c r="B37" t="s">
+      <c r="F37" t="s">
         <v>135</v>
       </c>
-      <c r="C37" t="s">
+      <c r="G37" t="s">
         <v>136</v>
       </c>
-      <c r="D37" t="s">
+      <c r="H37" t="s">
         <v>15</v>
       </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
         <v>137</v>
       </c>
-      <c r="B38" t="s">
+      <c r="F38" t="s">
         <v>138</v>
       </c>
-      <c r="C38" t="s">
+      <c r="G38" t="s">
         <v>139</v>
       </c>
-      <c r="D38" t="s">
+      <c r="H38" t="s">
         <v>140</v>
       </c>
-      <c r="E38">
+      <c r="I38">
         <v>13</v>
       </c>
-      <c r="F38" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="J38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
         <v>141</v>
       </c>
-      <c r="B39" t="s">
+      <c r="F39" t="s">
         <v>142</v>
       </c>
-      <c r="C39" t="s">
+      <c r="G39" t="s">
         <v>143</v>
       </c>
-      <c r="D39" t="s">
+      <c r="H39" t="s">
         <v>144</v>
       </c>
-      <c r="E39">
+      <c r="I39">
         <v>6</v>
       </c>
-      <c r="F39" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="J39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
         <v>145</v>
       </c>
-      <c r="B40" t="s">
+      <c r="F40" t="s">
         <v>146</v>
       </c>
-      <c r="C40" t="s">
+      <c r="G40" t="s">
         <v>147</v>
       </c>
-      <c r="D40" t="s">
+      <c r="H40" t="s">
         <v>148</v>
       </c>
-      <c r="E40">
+      <c r="I40">
         <v>5</v>
       </c>
-      <c r="F40" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="J40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
         <v>149</v>
       </c>
-      <c r="B41" t="s">
+      <c r="F41" t="s">
         <v>150</v>
       </c>
-      <c r="C41" t="s">
+      <c r="G41" t="s">
         <v>151</v>
       </c>
-      <c r="D41" t="s">
+      <c r="H41" t="s">
         <v>152</v>
       </c>
-      <c r="E41">
+      <c r="I41">
         <v>17</v>
       </c>
-      <c r="F41" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="J41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
         <v>153</v>
       </c>
-      <c r="B42" t="s">
+      <c r="F42" t="s">
         <v>154</v>
       </c>
-      <c r="C42" t="s">
+      <c r="G42" t="s">
         <v>155</v>
       </c>
-      <c r="D42" t="s">
+      <c r="H42" t="s">
         <v>39</v>
       </c>
-      <c r="E42">
+      <c r="I42">
         <v>2</v>
       </c>
-      <c r="F42" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
         <v>156</v>
       </c>
-      <c r="B43" t="s">
+      <c r="F43" t="s">
         <v>157</v>
       </c>
-      <c r="C43" t="s">
+      <c r="G43" t="s">
         <v>158</v>
       </c>
-      <c r="D43" t="s">
+      <c r="H43" t="s">
         <v>159</v>
       </c>
-      <c r="E43">
+      <c r="I43">
         <v>16</v>
       </c>
-      <c r="F43" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="J43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E44" t="s">
         <v>134</v>
       </c>
-      <c r="B44" t="s">
+      <c r="F44" t="s">
         <v>160</v>
       </c>
-      <c r="C44" t="s">
+      <c r="G44" t="s">
         <v>161</v>
       </c>
-      <c r="D44" t="s">
+      <c r="H44" t="s">
         <v>162</v>
       </c>
-      <c r="E44">
+      <c r="I44">
         <v>2</v>
       </c>
-      <c r="F44" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="J44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
         <v>163</v>
       </c>
-      <c r="B45" t="s">
+      <c r="F45" t="s">
         <v>164</v>
       </c>
-      <c r="C45" t="s">
+      <c r="G45" t="s">
         <v>165</v>
       </c>
-      <c r="D45" t="s">
+      <c r="H45" t="s">
         <v>166</v>
       </c>
-      <c r="E45">
+      <c r="I45">
         <v>4</v>
       </c>
-      <c r="F45" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="J45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E46" t="s">
         <v>167</v>
       </c>
-      <c r="B46" t="s">
+      <c r="F46" t="s">
         <v>168</v>
       </c>
-      <c r="C46" t="s">
+      <c r="G46" t="s">
         <v>169</v>
       </c>
-      <c r="D46" t="s">
+      <c r="H46" t="s">
         <v>170</v>
       </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
         <v>171</v>
       </c>
-      <c r="B47" t="s">
+      <c r="F47" t="s">
         <v>172</v>
       </c>
-      <c r="C47" t="s">
+      <c r="G47" t="s">
         <v>173</v>
       </c>
-      <c r="D47" t="s">
+      <c r="H47" t="s">
         <v>174</v>
       </c>
-      <c r="E47">
+      <c r="I47">
         <v>2</v>
       </c>
-      <c r="F47" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="J47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
         <v>175</v>
       </c>
-      <c r="B48" t="s">
+      <c r="F48" t="s">
         <v>176</v>
       </c>
-      <c r="C48" t="s">
+      <c r="G48" t="s">
         <v>177</v>
       </c>
-      <c r="D48" t="s">
+      <c r="H48" t="s">
         <v>178</v>
       </c>
-      <c r="E48">
+      <c r="I48">
         <v>6</v>
       </c>
-      <c r="F48" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="J48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E49" t="s">
         <v>179</v>
       </c>
-      <c r="B49" t="s">
+      <c r="F49" t="s">
         <v>180</v>
       </c>
-      <c r="C49" t="s">
+      <c r="G49" t="s">
         <v>181</v>
       </c>
-      <c r="D49" t="s">
+      <c r="H49" t="s">
         <v>144</v>
       </c>
-      <c r="E49">
+      <c r="I49">
         <v>20</v>
       </c>
-      <c r="F49" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="J49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
         <v>182</v>
       </c>
-      <c r="B50" t="s">
+      <c r="F50" t="s">
         <v>183</v>
       </c>
-      <c r="C50" t="s">
+      <c r="G50" t="s">
         <v>184</v>
       </c>
-      <c r="D50" t="s">
+      <c r="H50" t="s">
         <v>185</v>
       </c>
-      <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="J50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E51" t="s">
         <v>186</v>
       </c>
-      <c r="B51" t="s">
+      <c r="F51" t="s">
         <v>187</v>
       </c>
-      <c r="C51" t="s">
+      <c r="G51" t="s">
         <v>188</v>
       </c>
-      <c r="D51" t="s">
+      <c r="H51" t="s">
         <v>189</v>
       </c>
-      <c r="E51">
+      <c r="I51">
         <v>19</v>
       </c>
-      <c r="F51" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="J51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E52" t="s">
         <v>190</v>
       </c>
-      <c r="B52" t="s">
+      <c r="F52" t="s">
         <v>191</v>
       </c>
-      <c r="C52" t="s">
+      <c r="G52" t="s">
         <v>192</v>
       </c>
-      <c r="D52" t="s">
+      <c r="H52" t="s">
         <v>193</v>
       </c>
-      <c r="E52">
+      <c r="I52">
         <v>2</v>
       </c>
-      <c r="F52" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="J52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E53" t="s">
         <v>194</v>
       </c>
-      <c r="B53" t="s">
+      <c r="F53" t="s">
         <v>195</v>
       </c>
-      <c r="C53" t="s">
+      <c r="G53" t="s">
         <v>196</v>
       </c>
-      <c r="D53" t="s">
+      <c r="H53" t="s">
         <v>197</v>
       </c>
-      <c r="E53">
+      <c r="I53">
         <v>15</v>
       </c>
-      <c r="F53" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="J53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
         <v>198</v>
       </c>
-      <c r="B54" t="s">
+      <c r="F54" t="s">
         <v>199</v>
       </c>
-      <c r="C54" t="s">
+      <c r="G54" t="s">
         <v>200</v>
       </c>
-      <c r="D54" t="s">
+      <c r="H54" t="s">
         <v>201</v>
       </c>
-      <c r="E54">
+      <c r="I54">
         <v>20</v>
       </c>
-      <c r="F54" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="J54" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
         <v>202</v>
       </c>
-      <c r="B55" t="s">
+      <c r="F55" t="s">
         <v>203</v>
       </c>
-      <c r="C55" t="s">
+      <c r="G55" t="s">
         <v>204</v>
       </c>
-      <c r="D55" t="s">
+      <c r="H55" t="s">
         <v>205</v>
       </c>
-      <c r="E55">
+      <c r="I55">
         <v>10</v>
       </c>
-      <c r="F55" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="J55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
         <v>206</v>
       </c>
-      <c r="B56" t="s">
+      <c r="F56" t="s">
         <v>207</v>
       </c>
-      <c r="C56" t="s">
+      <c r="G56" t="s">
         <v>208</v>
       </c>
-      <c r="D56" t="s">
+      <c r="H56" t="s">
         <v>209</v>
       </c>
-      <c r="E56">
+      <c r="I56">
         <v>17</v>
       </c>
-      <c r="F56" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="J56" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
         <v>210</v>
       </c>
-      <c r="B57" t="s">
+      <c r="F57" t="s">
         <v>211</v>
       </c>
-      <c r="C57" t="s">
+      <c r="G57" t="s">
         <v>212</v>
       </c>
-      <c r="D57" t="s">
+      <c r="H57" t="s">
         <v>213</v>
       </c>
-      <c r="E57">
+      <c r="I57">
         <v>2</v>
       </c>
-      <c r="F57" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="J57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E58" t="s">
         <v>214</v>
       </c>
-      <c r="B58" t="s">
+      <c r="F58" t="s">
         <v>215</v>
       </c>
-      <c r="C58" t="s">
+      <c r="G58" t="s">
         <v>216</v>
       </c>
-      <c r="D58" t="s">
+      <c r="H58" t="s">
         <v>217</v>
       </c>
-      <c r="E58">
+      <c r="I58">
         <v>11</v>
       </c>
-      <c r="F58" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="J58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E59" t="s">
         <v>218</v>
       </c>
-      <c r="B59" t="s">
+      <c r="F59" t="s">
         <v>219</v>
       </c>
-      <c r="C59" t="s">
+      <c r="G59" t="s">
         <v>220</v>
       </c>
-      <c r="D59" t="s">
+      <c r="H59" t="s">
         <v>221</v>
       </c>
-      <c r="E59">
+      <c r="I59">
         <v>13</v>
       </c>
-      <c r="F59" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="J59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E60" t="s">
         <v>222</v>
       </c>
-      <c r="B60" t="s">
+      <c r="F60" t="s">
         <v>223</v>
       </c>
-      <c r="C60" t="s">
+      <c r="G60" t="s">
         <v>224</v>
       </c>
-      <c r="D60" t="s">
+      <c r="H60" t="s">
         <v>125</v>
       </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="F60" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E61" t="s">
         <v>225</v>
       </c>
-      <c r="B61" t="s">
+      <c r="F61" t="s">
         <v>226</v>
       </c>
-      <c r="C61" t="s">
+      <c r="G61" t="s">
         <v>227</v>
       </c>
-      <c r="D61" t="s">
+      <c r="H61" t="s">
         <v>228</v>
       </c>
-      <c r="E61">
+      <c r="I61">
         <v>9</v>
       </c>
-      <c r="F61" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="J61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E62" t="s">
         <v>229</v>
       </c>
-      <c r="B62" t="s">
+      <c r="F62" t="s">
         <v>230</v>
       </c>
-      <c r="C62" t="s">
+      <c r="G62" t="s">
         <v>231</v>
       </c>
-      <c r="D62" t="s">
+      <c r="H62" t="s">
         <v>232</v>
       </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="I62">
+        <v>1</v>
+      </c>
+      <c r="J62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E63" t="s">
         <v>233</v>
       </c>
-      <c r="B63" t="s">
+      <c r="F63" t="s">
         <v>234</v>
       </c>
-      <c r="C63" t="s">
+      <c r="G63" t="s">
         <v>235</v>
       </c>
-      <c r="D63" t="s">
+      <c r="H63" t="s">
         <v>236</v>
       </c>
-      <c r="E63">
+      <c r="I63">
         <v>3</v>
       </c>
-      <c r="F63" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="J63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E64" t="s">
         <v>237</v>
       </c>
-      <c r="B64" t="s">
+      <c r="F64" t="s">
         <v>238</v>
       </c>
-      <c r="C64" t="s">
+      <c r="G64" t="s">
         <v>239</v>
       </c>
-      <c r="D64" t="s">
+      <c r="H64" t="s">
         <v>95</v>
       </c>
-      <c r="E64">
+      <c r="I64">
         <v>18</v>
       </c>
-      <c r="F64" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="J64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E65" t="s">
         <v>240</v>
       </c>
-      <c r="B65" t="s">
+      <c r="F65" t="s">
         <v>241</v>
       </c>
-      <c r="C65" t="s">
+      <c r="G65" t="s">
         <v>242</v>
       </c>
-      <c r="D65" t="s">
+      <c r="H65" t="s">
         <v>243</v>
       </c>
-      <c r="E65">
+      <c r="I65">
         <v>8</v>
       </c>
-      <c r="F65" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="J65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E66" t="s">
         <v>244</v>
       </c>
-      <c r="B66" t="s">
+      <c r="F66" t="s">
         <v>245</v>
       </c>
-      <c r="C66" t="s">
+      <c r="G66" t="s">
         <v>246</v>
       </c>
-      <c r="D66" t="s">
+      <c r="H66" t="s">
         <v>247</v>
       </c>
-      <c r="E66">
+      <c r="I66">
         <v>7</v>
       </c>
-      <c r="F66" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="J66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E67" t="s">
         <v>248</v>
       </c>
-      <c r="B67" t="s">
+      <c r="F67" t="s">
         <v>249</v>
       </c>
-      <c r="C67" t="s">
+      <c r="G67" t="s">
         <v>250</v>
       </c>
-      <c r="D67" t="s">
+      <c r="H67" t="s">
         <v>251</v>
       </c>
-      <c r="E67">
-        <v>1</v>
-      </c>
-      <c r="F67" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="I67">
+        <v>1</v>
+      </c>
+      <c r="J67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E68" t="s">
         <v>252</v>
       </c>
-      <c r="B68" t="s">
+      <c r="F68" t="s">
         <v>253</v>
       </c>
-      <c r="C68" t="s">
+      <c r="G68" t="s">
         <v>254</v>
       </c>
-      <c r="D68" t="s">
+      <c r="H68" t="s">
         <v>217</v>
       </c>
-      <c r="E68">
+      <c r="I68">
         <v>7</v>
       </c>
-      <c r="F68" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="J68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E69" t="s">
         <v>255</v>
       </c>
-      <c r="B69" t="s">
+      <c r="F69" t="s">
         <v>256</v>
       </c>
-      <c r="C69" t="s">
+      <c r="G69" t="s">
         <v>257</v>
       </c>
-      <c r="D69" t="s">
+      <c r="H69" t="s">
         <v>258</v>
       </c>
-      <c r="E69">
+      <c r="I69">
         <v>17</v>
       </c>
-      <c r="F69" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="J69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E70" t="s">
         <v>259</v>
       </c>
-      <c r="B70" t="s">
+      <c r="F70" t="s">
         <v>260</v>
       </c>
-      <c r="C70" t="s">
+      <c r="G70" t="s">
         <v>261</v>
       </c>
-      <c r="D70" t="s">
+      <c r="H70" t="s">
         <v>262</v>
       </c>
-      <c r="E70">
+      <c r="I70">
         <v>6</v>
       </c>
-      <c r="F70" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="J70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
         <v>263</v>
       </c>
-      <c r="B71" t="s">
+      <c r="F71" t="s">
         <v>264</v>
       </c>
-      <c r="C71" t="s">
+      <c r="G71" t="s">
         <v>265</v>
       </c>
-      <c r="D71" t="s">
+      <c r="H71" t="s">
         <v>262</v>
       </c>
-      <c r="E71">
+      <c r="I71">
         <v>20</v>
       </c>
-      <c r="F71" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="J71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E72" t="s">
         <v>266</v>
       </c>
-      <c r="B72" t="s">
+      <c r="F72" t="s">
         <v>267</v>
       </c>
-      <c r="C72" t="s">
+      <c r="G72" t="s">
         <v>268</v>
       </c>
-      <c r="D72" t="s">
+      <c r="H72" t="s">
         <v>269</v>
       </c>
-      <c r="E72">
+      <c r="I72">
         <v>11</v>
       </c>
-      <c r="F72" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="J72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E73" t="s">
         <v>270</v>
       </c>
-      <c r="B73" t="s">
+      <c r="F73" t="s">
         <v>271</v>
       </c>
-      <c r="C73" t="s">
+      <c r="G73" t="s">
         <v>272</v>
       </c>
-      <c r="D73" t="s">
+      <c r="H73" t="s">
         <v>273</v>
       </c>
-      <c r="E73">
-        <v>1</v>
-      </c>
-      <c r="F73" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="I73">
+        <v>1</v>
+      </c>
+      <c r="J73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E74" t="s">
         <v>40</v>
       </c>
-      <c r="B74" t="s">
+      <c r="F74" t="s">
         <v>274</v>
       </c>
-      <c r="C74" t="s">
+      <c r="G74" t="s">
         <v>275</v>
       </c>
-      <c r="D74" t="s">
+      <c r="H74" t="s">
         <v>232</v>
       </c>
-      <c r="E74">
+      <c r="I74">
         <v>13</v>
       </c>
-      <c r="F74" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="J74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E75" t="s">
         <v>276</v>
       </c>
-      <c r="B75" t="s">
+      <c r="F75" t="s">
         <v>277</v>
       </c>
-      <c r="C75" t="s">
+      <c r="G75" t="s">
         <v>278</v>
       </c>
-      <c r="D75" t="s">
+      <c r="H75" t="s">
         <v>279</v>
       </c>
-      <c r="E75">
+      <c r="I75">
         <v>16</v>
       </c>
-      <c r="F75" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="J75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E76" t="s">
         <v>280</v>
       </c>
-      <c r="B76" t="s">
+      <c r="F76" t="s">
         <v>281</v>
       </c>
-      <c r="C76" t="s">
+      <c r="G76" t="s">
         <v>282</v>
       </c>
-      <c r="D76" t="s">
+      <c r="H76" t="s">
         <v>283</v>
       </c>
-      <c r="E76">
+      <c r="I76">
         <v>10</v>
       </c>
-      <c r="F76" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="J76" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E77" t="s">
         <v>284</v>
       </c>
-      <c r="B77" t="s">
+      <c r="F77" t="s">
         <v>285</v>
       </c>
-      <c r="C77" t="s">
+      <c r="G77" t="s">
         <v>286</v>
       </c>
-      <c r="D77" t="s">
+      <c r="H77" t="s">
         <v>189</v>
       </c>
-      <c r="E77">
+      <c r="I77">
         <v>13</v>
       </c>
-      <c r="F77" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="J77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E78" t="s">
         <v>287</v>
       </c>
-      <c r="B78" t="s">
+      <c r="F78" t="s">
         <v>288</v>
       </c>
-      <c r="C78" t="s">
+      <c r="G78" t="s">
         <v>289</v>
       </c>
-      <c r="D78" t="s">
+      <c r="H78" t="s">
         <v>290</v>
       </c>
-      <c r="E78">
+      <c r="I78">
         <v>8</v>
       </c>
-      <c r="F78" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="J78" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
         <v>291</v>
       </c>
-      <c r="B79" t="s">
+      <c r="F79" t="s">
         <v>292</v>
       </c>
-      <c r="C79" t="s">
+      <c r="G79" t="s">
         <v>293</v>
       </c>
-      <c r="D79" t="s">
+      <c r="H79" t="s">
         <v>294</v>
       </c>
-      <c r="E79">
+      <c r="I79">
         <v>7</v>
       </c>
-      <c r="F79" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="J79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
         <v>295</v>
       </c>
-      <c r="B80" t="s">
+      <c r="F80" t="s">
         <v>296</v>
       </c>
-      <c r="C80" t="s">
+      <c r="G80" t="s">
         <v>297</v>
       </c>
-      <c r="D80" t="s">
+      <c r="H80" t="s">
         <v>67</v>
       </c>
-      <c r="E80">
+      <c r="I80">
         <v>4</v>
       </c>
-      <c r="F80" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="J80" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
         <v>298</v>
       </c>
-      <c r="B81" t="s">
+      <c r="F81" t="s">
         <v>299</v>
       </c>
-      <c r="C81" t="s">
+      <c r="G81" t="s">
         <v>300</v>
       </c>
-      <c r="D81" t="s">
+      <c r="H81" t="s">
         <v>301</v>
       </c>
-      <c r="E81">
+      <c r="I81">
         <v>13</v>
       </c>
-      <c r="F81" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="J81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
         <v>302</v>
       </c>
-      <c r="B82" t="s">
+      <c r="F82" t="s">
         <v>303</v>
       </c>
-      <c r="C82" t="s">
+      <c r="G82" t="s">
         <v>304</v>
       </c>
-      <c r="D82" t="s">
+      <c r="H82" t="s">
         <v>305</v>
       </c>
-      <c r="E82">
+      <c r="I82">
         <v>17</v>
       </c>
-      <c r="F82" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="J82" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
         <v>306</v>
       </c>
-      <c r="B83" t="s">
+      <c r="F83" t="s">
         <v>307</v>
       </c>
-      <c r="C83" t="s">
+      <c r="G83" t="s">
         <v>308</v>
       </c>
-      <c r="D83" t="s">
+      <c r="H83" t="s">
         <v>309</v>
       </c>
-      <c r="E83">
+      <c r="I83">
         <v>12</v>
       </c>
-      <c r="F83" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="J83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
         <v>310</v>
       </c>
-      <c r="B84" t="s">
+      <c r="F84" t="s">
         <v>311</v>
       </c>
-      <c r="C84" t="s">
+      <c r="G84" t="s">
         <v>312</v>
       </c>
-      <c r="D84" t="s">
+      <c r="H84" t="s">
         <v>27</v>
       </c>
-      <c r="E84">
+      <c r="I84">
         <v>15</v>
       </c>
-      <c r="F84" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="J84" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
         <v>313</v>
       </c>
-      <c r="B85" t="s">
+      <c r="F85" t="s">
         <v>314</v>
       </c>
-      <c r="C85" t="s">
+      <c r="G85" t="s">
         <v>315</v>
       </c>
-      <c r="D85" t="s">
+      <c r="H85" t="s">
         <v>316</v>
       </c>
-      <c r="E85">
+      <c r="I85">
         <v>15</v>
       </c>
-      <c r="F85" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="J85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
         <v>317</v>
       </c>
-      <c r="B86" t="s">
+      <c r="F86" t="s">
         <v>318</v>
       </c>
-      <c r="C86" t="s">
+      <c r="G86" t="s">
         <v>319</v>
       </c>
-      <c r="D86" t="s">
+      <c r="H86" t="s">
         <v>320</v>
       </c>
-      <c r="E86">
+      <c r="I86">
         <v>19</v>
       </c>
-      <c r="F86" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="J86" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
         <v>321</v>
       </c>
-      <c r="B87" t="s">
+      <c r="F87" t="s">
         <v>322</v>
       </c>
-      <c r="C87" t="s">
+      <c r="G87" t="s">
         <v>323</v>
       </c>
-      <c r="D87" t="s">
+      <c r="H87" t="s">
         <v>324</v>
       </c>
-      <c r="E87">
+      <c r="I87">
         <v>12</v>
       </c>
-      <c r="F87" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="J87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
         <v>325</v>
       </c>
-      <c r="B88" t="s">
+      <c r="F88" t="s">
         <v>326</v>
       </c>
-      <c r="C88" t="s">
+      <c r="G88" t="s">
         <v>327</v>
       </c>
-      <c r="D88" t="s">
+      <c r="H88" t="s">
         <v>328</v>
       </c>
-      <c r="E88">
+      <c r="I88">
         <v>14</v>
       </c>
-      <c r="F88" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="J88" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
         <v>329</v>
       </c>
-      <c r="B89" t="s">
+      <c r="F89" t="s">
         <v>330</v>
       </c>
-      <c r="C89" t="s">
+      <c r="G89" t="s">
         <v>331</v>
       </c>
-      <c r="D89" t="s">
+      <c r="H89" t="s">
         <v>332</v>
       </c>
-      <c r="E89">
+      <c r="I89">
         <v>3</v>
       </c>
-      <c r="F89" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="J89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
         <v>333</v>
       </c>
-      <c r="B90" t="s">
+      <c r="F90" t="s">
         <v>334</v>
       </c>
-      <c r="C90" t="s">
+      <c r="G90" t="s">
         <v>335</v>
       </c>
-      <c r="D90" t="s">
+      <c r="H90" t="s">
         <v>336</v>
       </c>
-      <c r="E90">
+      <c r="I90">
         <v>2</v>
       </c>
-      <c r="F90" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="J90" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
         <v>337</v>
       </c>
-      <c r="B91" t="s">
+      <c r="F91" t="s">
         <v>338</v>
       </c>
-      <c r="C91" t="s">
+      <c r="G91" t="s">
         <v>339</v>
       </c>
-      <c r="D91" t="s">
+      <c r="H91" t="s">
         <v>340</v>
       </c>
-      <c r="E91">
+      <c r="I91">
         <v>2</v>
       </c>
-      <c r="F91" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="J91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
         <v>341</v>
       </c>
-      <c r="B92" t="s">
+      <c r="F92" t="s">
         <v>342</v>
       </c>
-      <c r="C92" t="s">
+      <c r="G92" t="s">
         <v>343</v>
       </c>
-      <c r="D92" t="s">
+      <c r="H92" t="s">
         <v>123</v>
       </c>
-      <c r="E92">
+      <c r="I92">
         <v>16</v>
       </c>
-      <c r="F92" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="J92" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
         <v>344</v>
       </c>
-      <c r="B93" t="s">
+      <c r="F93" t="s">
         <v>345</v>
       </c>
-      <c r="C93" t="s">
+      <c r="G93" t="s">
         <v>346</v>
       </c>
-      <c r="D93" t="s">
+      <c r="H93" t="s">
         <v>144</v>
       </c>
-      <c r="E93">
+      <c r="I93">
         <v>19</v>
       </c>
-      <c r="F93" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="J93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E94" t="s">
         <v>347</v>
       </c>
-      <c r="B94" t="s">
+      <c r="F94" t="s">
         <v>348</v>
       </c>
-      <c r="C94" t="s">
+      <c r="G94" t="s">
         <v>349</v>
       </c>
-      <c r="D94" t="s">
+      <c r="H94" t="s">
         <v>350</v>
       </c>
-      <c r="E94">
+      <c r="I94">
         <v>9</v>
       </c>
-      <c r="F94" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="J94" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E95" t="s">
         <v>351</v>
       </c>
-      <c r="B95" t="s">
+      <c r="F95" t="s">
         <v>352</v>
       </c>
-      <c r="C95" t="s">
+      <c r="G95" t="s">
         <v>353</v>
       </c>
-      <c r="D95" t="s">
+      <c r="H95" t="s">
         <v>350</v>
       </c>
-      <c r="E95">
+      <c r="I95">
         <v>10</v>
       </c>
-      <c r="F95" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="J95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E96" t="s">
         <v>354</v>
       </c>
-      <c r="B96" t="s">
+      <c r="F96" t="s">
         <v>355</v>
       </c>
-      <c r="C96" t="s">
+      <c r="G96" t="s">
         <v>356</v>
       </c>
-      <c r="D96" t="s">
+      <c r="H96" t="s">
         <v>357</v>
       </c>
-      <c r="E96">
-        <v>1</v>
-      </c>
-      <c r="F96" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="I96">
+        <v>1</v>
+      </c>
+      <c r="J96" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E97" t="s">
         <v>358</v>
       </c>
-      <c r="B97" t="s">
+      <c r="F97" t="s">
         <v>359</v>
       </c>
-      <c r="C97" t="s">
+      <c r="G97" t="s">
         <v>360</v>
       </c>
-      <c r="D97" t="s">
+      <c r="H97" t="s">
         <v>361</v>
       </c>
-      <c r="E97">
-        <v>1</v>
-      </c>
-      <c r="F97" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="I97">
+        <v>1</v>
+      </c>
+      <c r="J97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E98" t="s">
         <v>362</v>
       </c>
-      <c r="B98" t="s">
+      <c r="F98" t="s">
         <v>363</v>
       </c>
-      <c r="C98" t="s">
+      <c r="G98" t="s">
         <v>364</v>
       </c>
-      <c r="D98" t="s">
+      <c r="H98" t="s">
         <v>365</v>
       </c>
-      <c r="E98">
+      <c r="I98">
         <v>2</v>
       </c>
-      <c r="F98" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="J98" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E99" t="s">
         <v>366</v>
       </c>
-      <c r="B99" t="s">
+      <c r="F99" t="s">
         <v>367</v>
       </c>
-      <c r="C99" t="s">
+      <c r="G99" t="s">
         <v>368</v>
       </c>
-      <c r="D99" t="s">
+      <c r="H99" t="s">
         <v>369</v>
       </c>
-      <c r="E99">
+      <c r="I99">
         <v>19</v>
       </c>
-      <c r="F99" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="J99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E100" t="s">
         <v>370</v>
       </c>
-      <c r="B100" t="s">
+      <c r="F100" t="s">
         <v>371</v>
       </c>
-      <c r="C100" t="s">
+      <c r="G100" t="s">
         <v>372</v>
       </c>
-      <c r="D100" t="s">
+      <c r="H100" t="s">
         <v>373</v>
       </c>
-      <c r="E100">
+      <c r="I100">
         <v>16</v>
       </c>
-      <c r="F100" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="J100" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E101" t="s">
         <v>374</v>
       </c>
-      <c r="B101" t="s">
+      <c r="F101" t="s">
         <v>375</v>
       </c>
-      <c r="C101" t="s">
+      <c r="G101" t="s">
         <v>376</v>
       </c>
-      <c r="D101" t="s">
+      <c r="H101" t="s">
         <v>377</v>
       </c>
-      <c r="E101">
-        <v>1</v>
-      </c>
-      <c r="F101" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="I101">
+        <v>1</v>
+      </c>
+      <c r="J101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
         <v>378</v>
       </c>
-      <c r="B102" t="s">
+      <c r="F102" t="s">
         <v>379</v>
       </c>
-      <c r="C102" t="s">
+      <c r="G102" t="s">
         <v>380</v>
       </c>
-      <c r="D102" t="s">
+      <c r="H102" t="s">
         <v>381</v>
       </c>
-      <c r="E102">
+      <c r="I102">
         <v>8</v>
       </c>
-      <c r="F102" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="J102" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E103" t="s">
         <v>382</v>
       </c>
-      <c r="B103" t="s">
+      <c r="F103" t="s">
         <v>383</v>
       </c>
-      <c r="C103" t="s">
+      <c r="G103" t="s">
         <v>384</v>
       </c>
-      <c r="D103" t="s">
+      <c r="H103" t="s">
         <v>15</v>
       </c>
-      <c r="E103">
+      <c r="I103">
         <v>13</v>
       </c>
-      <c r="F103" t="b">
+      <c r="J103" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Added capability to continue/stop after encountering blank row - Added capability to include/skip blank rows
Signed-off-by: LeandroC89 <leandroadao3@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/krangl/data/ExcelReadExample.xlsx
+++ b/src/test/resources/krangl/data/ExcelReadExample.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LCouto\IdeaProjects\krangl\src\test\resources\krangl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711EC427-5760-4F92-BEAA-E4D4075BEA04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69976BA-D69F-489E-A444-3CCB68B6AC15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22530" yWindow="-4230" windowWidth="17760" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstSheet" sheetId="1" r:id="rId1"/>
     <sheet name="SecondSheet" sheetId="2" r:id="rId2"/>
+    <sheet name="ThirdSheet" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="390">
   <si>
     <t>Name</t>
   </si>
@@ -1234,9 +1235,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1543,7 +1545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3580,8 +3582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D48153-1644-422E-BF6C-88BBA322D82D}">
   <dimension ref="E3:J103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5614,4 +5616,177 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF8BC6C-5E1D-4BA0-91B9-450DCF6DAEB9}">
+  <dimension ref="E3:J10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="4" width="9.140625" style="2"/>
+    <col min="5" max="5" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>385</v>
+      </c>
+      <c r="J3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="4" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <v>20</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5">
+        <v>17</v>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>387</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6">
+        <v>14</v>
+      </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7">
+        <v>10</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>388</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I9">
+        <v>18</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Adjusted Excel read file to properly test line skips
Signed-off-by: LeandroC89 <leandroadao3@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/krangl/data/ExcelReadExample.xlsx
+++ b/src/test/resources/krangl/data/ExcelReadExample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LCouto\IdeaProjects\krangl\src\test\resources\krangl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB32BCB-89F2-4EAD-989B-EA03298765B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9645B304-D1B9-4DEF-BC72-AC2D7C6EF2D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5115" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-5115" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstSheet" sheetId="1" r:id="rId1"/>
@@ -3583,10 +3583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D48153-1644-422E-BF6C-88BBA322D82D}">
-  <dimension ref="E3:J103"/>
+  <dimension ref="E5:J105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3599,141 +3599,101 @@
     <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" t="s">
-        <v>385</v>
-      </c>
-      <c r="J3" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="4" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4">
-        <v>20</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-    </row>
     <row r="5" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5">
-        <v>17</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>385</v>
+      </c>
+      <c r="J5" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="6" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>387</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="I6">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7">
         <v>17</v>
       </c>
-      <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7">
-        <v>10</v>
-      </c>
       <c r="J7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
-        <v>20</v>
+        <v>387</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="J8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
-        <v>388</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="H9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="I9">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="J9" t="b">
         <v>0</v>
@@ -3741,16 +3701,16 @@
     </row>
     <row r="10" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -3761,19 +3721,19 @@
     </row>
     <row r="11" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>32</v>
+        <v>388</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="H11" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="I11">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J11" t="b">
         <v>0</v>
@@ -3781,19 +3741,19 @@
     </row>
     <row r="12" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="G12" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="H12" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="I12">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J12" t="b">
         <v>1</v>
@@ -3801,19 +3761,19 @@
     </row>
     <row r="13" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G13" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H13" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="I13">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="J13" t="b">
         <v>0</v>
@@ -3821,19 +3781,19 @@
     </row>
     <row r="14" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G14" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="I14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
@@ -3841,19 +3801,19 @@
     </row>
     <row r="15" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="G15" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H15" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J15" t="b">
         <v>0</v>
@@ -3861,19 +3821,19 @@
     </row>
     <row r="16" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G16" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="H16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="I16">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="J16" t="b">
         <v>1</v>
@@ -3881,19 +3841,19 @@
     </row>
     <row r="17" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E17" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H17" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J17" t="b">
         <v>0</v>
@@ -3901,19 +3861,19 @@
     </row>
     <row r="18" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G18" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="I18">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
@@ -3921,19 +3881,19 @@
     </row>
     <row r="19" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="G19" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H19" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="I19">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J19" t="b">
         <v>0</v>
@@ -3941,19 +3901,19 @@
     </row>
     <row r="20" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F20" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="H20" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="I20">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="J20" t="b">
         <v>1</v>
@@ -3961,19 +3921,19 @@
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="F21" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H21" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="I21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J21" t="b">
         <v>0</v>
@@ -3981,19 +3941,19 @@
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F22" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="G22" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="I22">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J22" t="b">
         <v>1</v>
@@ -4001,19 +3961,19 @@
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F23" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H23" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I23">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J23" t="b">
         <v>0</v>
@@ -4021,19 +3981,19 @@
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="F24" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="G24" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H24" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="I24">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="J24" t="b">
         <v>1</v>
@@ -4041,19 +4001,19 @@
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="F25" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="G25" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="H25" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="I25">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J25" t="b">
         <v>0</v>
@@ -4061,19 +4021,19 @@
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F26" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G26" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="H26" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="I26">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J26" t="b">
         <v>1</v>
@@ -4081,19 +4041,19 @@
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F27" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G27" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="H27" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I27">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="J27" t="b">
         <v>0</v>
@@ -4101,19 +4061,19 @@
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F28" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G28" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="H28" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="I28">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J28" t="b">
         <v>1</v>
@@ -4121,19 +4081,19 @@
     </row>
     <row r="29" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="F29" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G29" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H29" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="I29">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="J29" t="b">
         <v>0</v>
@@ -4141,19 +4101,19 @@
     </row>
     <row r="30" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F30" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="G30" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="H30" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="I30">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J30" t="b">
         <v>1</v>
@@ -4161,19 +4121,19 @@
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="F31" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="G31" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="H31" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="J31" t="b">
         <v>0</v>
@@ -4181,19 +4141,19 @@
     </row>
     <row r="32" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="F32" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="G32" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="H32" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="I32">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J32" t="b">
         <v>1</v>
@@ -4201,19 +4161,19 @@
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F33" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="G33" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="H33" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="I33">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="J33" t="b">
         <v>0</v>
@@ -4221,16 +4181,19 @@
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>389</v>
+        <v>116</v>
+      </c>
+      <c r="F34" t="s">
+        <v>117</v>
       </c>
       <c r="G34" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="H34" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="I34">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J34" t="b">
         <v>1</v>
@@ -4238,19 +4201,19 @@
     </row>
     <row r="35" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="F35" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="G35" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H35" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="I35">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="J35" t="b">
         <v>0</v>
@@ -4258,19 +4221,16 @@
     </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
-        <v>130</v>
-      </c>
-      <c r="F36" t="s">
-        <v>131</v>
+        <v>389</v>
       </c>
       <c r="G36" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H36" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="I36">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J36" t="b">
         <v>1</v>
@@ -4278,19 +4238,19 @@
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="F37" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G37" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="H37" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J37" t="b">
         <v>0</v>
@@ -4298,19 +4258,19 @@
     </row>
     <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F38" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="G38" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="H38" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="I38">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J38" t="b">
         <v>1</v>
@@ -4318,19 +4278,19 @@
     </row>
     <row r="39" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="F39" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="G39" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="H39" t="s">
-        <v>144</v>
+        <v>15</v>
       </c>
       <c r="I39">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J39" t="b">
         <v>0</v>
@@ -4338,19 +4298,19 @@
     </row>
     <row r="40" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="F40" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="G40" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H40" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="I40">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="J40" t="b">
         <v>1</v>
@@ -4358,19 +4318,19 @@
     </row>
     <row r="41" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F41" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G41" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="H41" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I41">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="J41" t="b">
         <v>0</v>
@@ -4378,19 +4338,19 @@
     </row>
     <row r="42" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="F42" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="G42" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="H42" t="s">
-        <v>39</v>
+        <v>148</v>
       </c>
       <c r="I42">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J42" t="b">
         <v>1</v>
@@ -4398,19 +4358,19 @@
     </row>
     <row r="43" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E43" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="F43" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="G43" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="H43" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="I43">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J43" t="b">
         <v>0</v>
@@ -4418,16 +4378,16 @@
     </row>
     <row r="44" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="F44" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G44" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="H44" t="s">
-        <v>162</v>
+        <v>39</v>
       </c>
       <c r="I44">
         <v>2</v>
@@ -4438,19 +4398,19 @@
     </row>
     <row r="45" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="F45" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="G45" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="H45" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="I45">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="J45" t="b">
         <v>0</v>
@@ -4458,19 +4418,19 @@
     </row>
     <row r="46" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E46" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="F46" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="G46" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="H46" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J46" t="b">
         <v>1</v>
@@ -4478,19 +4438,19 @@
     </row>
     <row r="47" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="F47" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="G47" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="H47" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="I47">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J47" t="b">
         <v>0</v>
@@ -4498,19 +4458,19 @@
     </row>
     <row r="48" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F48" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G48" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="H48" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="I48">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="J48" t="b">
         <v>1</v>
@@ -4518,19 +4478,19 @@
     </row>
     <row r="49" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F49" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G49" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="H49" t="s">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="I49">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="J49" t="b">
         <v>0</v>
@@ -4538,19 +4498,19 @@
     </row>
     <row r="50" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E50" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="F50" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="G50" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="H50" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="I50">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J50" t="b">
         <v>1</v>
@@ -4558,19 +4518,19 @@
     </row>
     <row r="51" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E51" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="F51" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="G51" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="H51" t="s">
-        <v>189</v>
+        <v>144</v>
       </c>
       <c r="I51">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J51" t="b">
         <v>0</v>
@@ -4578,19 +4538,19 @@
     </row>
     <row r="52" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="F52" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="G52" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="H52" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="I52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J52" t="b">
         <v>1</v>
@@ -4598,19 +4558,19 @@
     </row>
     <row r="53" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="F53" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="G53" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="H53" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="I53">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="J53" t="b">
         <v>0</v>
@@ -4618,19 +4578,19 @@
     </row>
     <row r="54" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F54" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="G54" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="H54" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="I54">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="J54" t="b">
         <v>1</v>
@@ -4638,19 +4598,19 @@
     </row>
     <row r="55" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="F55" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="G55" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="H55" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="I55">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="J55" t="b">
         <v>0</v>
@@ -4658,19 +4618,19 @@
     </row>
     <row r="56" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="F56" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="G56" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="H56" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="I56">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J56" t="b">
         <v>1</v>
@@ -4678,19 +4638,19 @@
     </row>
     <row r="57" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="F57" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="G57" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H57" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="I57">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="J57" t="b">
         <v>0</v>
@@ -4698,19 +4658,19 @@
     </row>
     <row r="58" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E58" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="F58" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="G58" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="H58" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="I58">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J58" t="b">
         <v>1</v>
@@ -4718,19 +4678,19 @@
     </row>
     <row r="59" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E59" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="F59" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="G59" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="H59" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="I59">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="J59" t="b">
         <v>0</v>
@@ -4738,19 +4698,19 @@
     </row>
     <row r="60" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="F60" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="G60" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="H60" t="s">
-        <v>125</v>
+        <v>217</v>
       </c>
       <c r="I60">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="J60" t="b">
         <v>1</v>
@@ -4758,19 +4718,19 @@
     </row>
     <row r="61" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="F61" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G61" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="H61" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="I61">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J61" t="b">
         <v>0</v>
@@ -4778,16 +4738,16 @@
     </row>
     <row r="62" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="F62" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="G62" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="H62" t="s">
-        <v>232</v>
+        <v>125</v>
       </c>
       <c r="I62">
         <v>1</v>
@@ -4798,19 +4758,19 @@
     </row>
     <row r="63" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="F63" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="G63" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="H63" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="I63">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J63" t="b">
         <v>0</v>
@@ -4818,19 +4778,19 @@
     </row>
     <row r="64" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="F64" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="G64" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="H64" t="s">
-        <v>95</v>
+        <v>232</v>
       </c>
       <c r="I64">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="J64" t="b">
         <v>1</v>
@@ -4838,19 +4798,19 @@
     </row>
     <row r="65" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F65" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="G65" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="H65" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="I65">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="J65" t="b">
         <v>0</v>
@@ -4858,19 +4818,19 @@
     </row>
     <row r="66" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="F66" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="G66" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="H66" t="s">
-        <v>247</v>
+        <v>95</v>
       </c>
       <c r="I66">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="J66" t="b">
         <v>1</v>
@@ -4878,19 +4838,19 @@
     </row>
     <row r="67" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E67" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="F67" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="G67" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="H67" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="I67">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J67" t="b">
         <v>0</v>
@@ -4898,16 +4858,16 @@
     </row>
     <row r="68" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="F68" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G68" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="H68" t="s">
-        <v>217</v>
+        <v>247</v>
       </c>
       <c r="I68">
         <v>7</v>
@@ -4918,19 +4878,19 @@
     </row>
     <row r="69" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="F69" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="G69" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="H69" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="I69">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="J69" t="b">
         <v>0</v>
@@ -4938,19 +4898,19 @@
     </row>
     <row r="70" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F70" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="G70" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="H70" t="s">
-        <v>262</v>
+        <v>217</v>
       </c>
       <c r="I70">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J70" t="b">
         <v>1</v>
@@ -4958,19 +4918,19 @@
     </row>
     <row r="71" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E71" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="F71" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="G71" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="H71" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="I71">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="J71" t="b">
         <v>0</v>
@@ -4978,19 +4938,19 @@
     </row>
     <row r="72" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E72" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="F72" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="G72" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="H72" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="I72">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="J72" t="b">
         <v>1</v>
@@ -4998,19 +4958,19 @@
     </row>
     <row r="73" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="F73" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="G73" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="H73" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="I73">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J73" t="b">
         <v>0</v>
@@ -5018,19 +4978,19 @@
     </row>
     <row r="74" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E74" t="s">
-        <v>40</v>
+        <v>266</v>
       </c>
       <c r="F74" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="G74" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="H74" t="s">
-        <v>232</v>
+        <v>269</v>
       </c>
       <c r="I74">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J74" t="b">
         <v>1</v>
@@ -5038,19 +4998,19 @@
     </row>
     <row r="75" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="F75" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="G75" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="H75" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="I75">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="J75" t="b">
         <v>0</v>
@@ -5058,19 +5018,19 @@
     </row>
     <row r="76" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
-        <v>280</v>
+        <v>40</v>
       </c>
       <c r="F76" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="G76" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="H76" t="s">
-        <v>283</v>
+        <v>232</v>
       </c>
       <c r="I76">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J76" t="b">
         <v>1</v>
@@ -5078,19 +5038,19 @@
     </row>
     <row r="77" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E77" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="F77" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="G77" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="H77" t="s">
-        <v>189</v>
+        <v>279</v>
       </c>
       <c r="I77">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="J77" t="b">
         <v>0</v>
@@ -5098,19 +5058,19 @@
     </row>
     <row r="78" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="F78" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G78" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="H78" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="I78">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J78" t="b">
         <v>1</v>
@@ -5118,19 +5078,19 @@
     </row>
     <row r="79" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="F79" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="G79" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="H79" t="s">
-        <v>294</v>
+        <v>189</v>
       </c>
       <c r="I79">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="J79" t="b">
         <v>0</v>
@@ -5138,19 +5098,19 @@
     </row>
     <row r="80" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E80" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="F80" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="G80" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="H80" t="s">
-        <v>67</v>
+        <v>290</v>
       </c>
       <c r="I80">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J80" t="b">
         <v>1</v>
@@ -5158,19 +5118,19 @@
     </row>
     <row r="81" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="F81" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="G81" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="H81" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="I81">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="J81" t="b">
         <v>0</v>
@@ -5178,19 +5138,19 @@
     </row>
     <row r="82" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E82" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="F82" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="G82" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="H82" t="s">
-        <v>305</v>
+        <v>67</v>
       </c>
       <c r="I82">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="J82" t="b">
         <v>1</v>
@@ -5198,19 +5158,19 @@
     </row>
     <row r="83" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="F83" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="G83" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="H83" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="I83">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="J83" t="b">
         <v>0</v>
@@ -5218,19 +5178,19 @@
     </row>
     <row r="84" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E84" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="F84" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="G84" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="H84" t="s">
-        <v>27</v>
+        <v>305</v>
       </c>
       <c r="I84">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="J84" t="b">
         <v>1</v>
@@ -5238,19 +5198,19 @@
     </row>
     <row r="85" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E85" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="F85" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="G85" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="H85" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="I85">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J85" t="b">
         <v>0</v>
@@ -5258,19 +5218,19 @@
     </row>
     <row r="86" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E86" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="F86" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="G86" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="H86" t="s">
-        <v>320</v>
+        <v>27</v>
       </c>
       <c r="I86">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J86" t="b">
         <v>1</v>
@@ -5278,19 +5238,19 @@
     </row>
     <row r="87" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E87" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="F87" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="G87" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="H87" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="I87">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J87" t="b">
         <v>0</v>
@@ -5298,19 +5258,19 @@
     </row>
     <row r="88" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E88" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="F88" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="G88" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="H88" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="I88">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J88" t="b">
         <v>1</v>
@@ -5318,19 +5278,19 @@
     </row>
     <row r="89" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E89" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="F89" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="G89" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="H89" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="I89">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="J89" t="b">
         <v>0</v>
@@ -5338,19 +5298,19 @@
     </row>
     <row r="90" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E90" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="F90" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="G90" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="H90" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="I90">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="J90" t="b">
         <v>1</v>
@@ -5358,19 +5318,19 @@
     </row>
     <row r="91" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E91" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="F91" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="G91" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="H91" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="I91">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J91" t="b">
         <v>0</v>
@@ -5378,19 +5338,19 @@
     </row>
     <row r="92" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E92" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="F92" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="G92" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="H92" t="s">
-        <v>123</v>
+        <v>336</v>
       </c>
       <c r="I92">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="J92" t="b">
         <v>1</v>
@@ -5398,19 +5358,19 @@
     </row>
     <row r="93" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E93" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="F93" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="G93" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="H93" t="s">
-        <v>144</v>
+        <v>340</v>
       </c>
       <c r="I93">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="J93" t="b">
         <v>0</v>
@@ -5418,19 +5378,19 @@
     </row>
     <row r="94" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E94" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="F94" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="G94" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="H94" t="s">
-        <v>350</v>
+        <v>123</v>
       </c>
       <c r="I94">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J94" t="b">
         <v>1</v>
@@ -5438,19 +5398,19 @@
     </row>
     <row r="95" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E95" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="F95" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="G95" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="H95" t="s">
-        <v>350</v>
+        <v>144</v>
       </c>
       <c r="I95">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="J95" t="b">
         <v>0</v>
@@ -5458,19 +5418,19 @@
     </row>
     <row r="96" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E96" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="F96" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="G96" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="H96" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="I96">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J96" t="b">
         <v>1</v>
@@ -5478,19 +5438,19 @@
     </row>
     <row r="97" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E97" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="F97" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="G97" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="H97" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="I97">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J97" t="b">
         <v>0</v>
@@ -5498,19 +5458,19 @@
     </row>
     <row r="98" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E98" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="F98" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="G98" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="H98" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="I98">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J98" t="b">
         <v>1</v>
@@ -5518,19 +5478,19 @@
     </row>
     <row r="99" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E99" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="F99" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="G99" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="H99" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="I99">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="J99" t="b">
         <v>0</v>
@@ -5538,19 +5498,19 @@
     </row>
     <row r="100" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E100" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="F100" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="G100" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="H100" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="I100">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="J100" t="b">
         <v>1</v>
@@ -5558,19 +5518,19 @@
     </row>
     <row r="101" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E101" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="F101" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="G101" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="H101" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="I101">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="J101" t="b">
         <v>0</v>
@@ -5578,19 +5538,19 @@
     </row>
     <row r="102" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E102" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="F102" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="G102" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="H102" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="I102">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J102" t="b">
         <v>1</v>
@@ -5598,21 +5558,61 @@
     </row>
     <row r="103" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E103" t="s">
+        <v>374</v>
+      </c>
+      <c r="F103" t="s">
+        <v>375</v>
+      </c>
+      <c r="G103" t="s">
+        <v>376</v>
+      </c>
+      <c r="H103" t="s">
+        <v>377</v>
+      </c>
+      <c r="I103">
+        <v>1</v>
+      </c>
+      <c r="J103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E104" t="s">
+        <v>378</v>
+      </c>
+      <c r="F104" t="s">
+        <v>379</v>
+      </c>
+      <c r="G104" t="s">
+        <v>380</v>
+      </c>
+      <c r="H104" t="s">
+        <v>381</v>
+      </c>
+      <c r="I104">
+        <v>8</v>
+      </c>
+      <c r="J104" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E105" t="s">
         <v>382</v>
       </c>
-      <c r="F103" t="s">
+      <c r="F105" t="s">
         <v>383</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G105" t="s">
         <v>384</v>
       </c>
-      <c r="H103" t="s">
+      <c r="H105" t="s">
         <v>15</v>
       </c>
-      <c r="I103">
+      <c r="I105">
         <v>13</v>
       </c>
-      <c r="J103" t="b">
+      <c r="J105" t="b">
         <v>0</v>
       </c>
     </row>
@@ -5625,7 +5625,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF8BC6C-5E1D-4BA0-91B9-450DCF6DAEB9}">
   <dimension ref="D3:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Use toLong in order to support large numeric values
</commit_message>
<xml_diff>
--- a/src/test/resources/krangl/data/ExcelReadExample.xlsx
+++ b/src/test/resources/krangl/data/ExcelReadExample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10509"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\misc\krangl\src\test\resources\krangl\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayvazj/src/krangl/src/test/resources/krangl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CA1C79-D1D3-40F1-9715-2C7B9842002D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B9CE83-F4E2-3844-9096-95018DA6CCAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15945" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstSheet" sheetId="1" r:id="rId1"/>
@@ -1234,7 +1234,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -1539,18 +1539,19 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1570,7 +1571,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1590,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1604,13 +1605,13 @@
         <v>11</v>
       </c>
       <c r="E3">
-        <v>17</v>
+        <v>432178937489174</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1630,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1650,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1670,7 +1671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1707,7 +1708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1727,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1747,7 +1748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1767,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -1787,7 +1788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1807,7 +1808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1827,7 +1828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1847,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1867,7 +1868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1907,7 +1908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -1927,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>76</v>
       </c>
@@ -1947,7 +1948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -1967,7 +1968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>84</v>
       </c>
@@ -1987,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>88</v>
       </c>
@@ -2007,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -2027,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -2047,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>100</v>
       </c>
@@ -2067,7 +2068,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>104</v>
       </c>
@@ -2087,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>108</v>
       </c>
@@ -2107,7 +2108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>112</v>
       </c>
@@ -2127,7 +2128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -2147,7 +2148,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>120</v>
       </c>
@@ -2167,7 +2168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>389</v>
       </c>
@@ -2184,7 +2185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>126</v>
       </c>
@@ -2204,7 +2205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>130</v>
       </c>
@@ -2224,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>134</v>
       </c>
@@ -2244,7 +2245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>137</v>
       </c>
@@ -2264,7 +2265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>141</v>
       </c>
@@ -2284,7 +2285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -2304,7 +2305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -2324,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>153</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>156</v>
       </c>
@@ -2364,7 +2365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>134</v>
       </c>
@@ -2384,7 +2385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>163</v>
       </c>
@@ -2404,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>167</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>171</v>
       </c>
@@ -2444,7 +2445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>175</v>
       </c>
@@ -2464,7 +2465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>179</v>
       </c>
@@ -2484,7 +2485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>182</v>
       </c>
@@ -2504,7 +2505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>186</v>
       </c>
@@ -2524,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>190</v>
       </c>
@@ -2544,7 +2545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>194</v>
       </c>
@@ -2564,7 +2565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>198</v>
       </c>
@@ -2584,7 +2585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>202</v>
       </c>
@@ -2604,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>206</v>
       </c>
@@ -2624,7 +2625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>210</v>
       </c>
@@ -2644,7 +2645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>214</v>
       </c>
@@ -2664,7 +2665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>218</v>
       </c>
@@ -2684,7 +2685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>222</v>
       </c>
@@ -2704,7 +2705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>225</v>
       </c>
@@ -2724,7 +2725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>229</v>
       </c>
@@ -2744,7 +2745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>233</v>
       </c>
@@ -2764,7 +2765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>237</v>
       </c>
@@ -2784,7 +2785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>240</v>
       </c>
@@ -2804,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>244</v>
       </c>
@@ -2824,7 +2825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>248</v>
       </c>
@@ -2844,7 +2845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>252</v>
       </c>
@@ -2864,7 +2865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>255</v>
       </c>
@@ -2884,7 +2885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>259</v>
       </c>
@@ -2904,7 +2905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>263</v>
       </c>
@@ -2924,7 +2925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>266</v>
       </c>
@@ -2944,7 +2945,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>270</v>
       </c>
@@ -2964,7 +2965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>40</v>
       </c>
@@ -2984,7 +2985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>276</v>
       </c>
@@ -3004,7 +3005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>280</v>
       </c>
@@ -3024,7 +3025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>284</v>
       </c>
@@ -3044,7 +3045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>287</v>
       </c>
@@ -3064,7 +3065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>291</v>
       </c>
@@ -3084,7 +3085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>295</v>
       </c>
@@ -3104,7 +3105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>298</v>
       </c>
@@ -3124,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>302</v>
       </c>
@@ -3144,7 +3145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>306</v>
       </c>
@@ -3164,7 +3165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>310</v>
       </c>
@@ -3184,7 +3185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>313</v>
       </c>
@@ -3204,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>317</v>
       </c>
@@ -3224,7 +3225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>321</v>
       </c>
@@ -3244,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>325</v>
       </c>
@@ -3264,7 +3265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>329</v>
       </c>
@@ -3284,7 +3285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>333</v>
       </c>
@@ -3304,7 +3305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>337</v>
       </c>
@@ -3324,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>341</v>
       </c>
@@ -3344,7 +3345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>344</v>
       </c>
@@ -3364,7 +3365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>347</v>
       </c>
@@ -3384,7 +3385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>351</v>
       </c>
@@ -3404,7 +3405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>354</v>
       </c>
@@ -3424,7 +3425,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>358</v>
       </c>
@@ -3444,7 +3445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>362</v>
       </c>
@@ -3464,7 +3465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>366</v>
       </c>
@@ -3484,7 +3485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>370</v>
       </c>
@@ -3504,7 +3505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>374</v>
       </c>
@@ -3524,7 +3525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>378</v>
       </c>
@@ -3544,7 +3545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>382</v>
       </c>
@@ -3567,6 +3568,7 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -3575,20 +3577,20 @@
   <dimension ref="E5:J105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="46.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>0</v>
       </c>
@@ -3608,7 +3610,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="6" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>4</v>
       </c>
@@ -3628,7 +3630,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>8</v>
       </c>
@@ -3642,13 +3644,13 @@
         <v>11</v>
       </c>
       <c r="I7">
-        <v>17</v>
+        <v>432178937489174</v>
       </c>
       <c r="J7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>387</v>
       </c>
@@ -3668,7 +3670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>16</v>
       </c>
@@ -3688,7 +3690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>20</v>
       </c>
@@ -3708,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>388</v>
       </c>
@@ -3725,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>28</v>
       </c>
@@ -3745,7 +3747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
         <v>32</v>
       </c>
@@ -3765,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
         <v>36</v>
       </c>
@@ -3785,7 +3787,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
         <v>40</v>
       </c>
@@ -3805,7 +3807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
         <v>44</v>
       </c>
@@ -3825,7 +3827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>48</v>
       </c>
@@ -3845,7 +3847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>52</v>
       </c>
@@ -3865,7 +3867,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
         <v>56</v>
       </c>
@@ -3885,7 +3887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
         <v>60</v>
       </c>
@@ -3905,7 +3907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
         <v>64</v>
       </c>
@@ -3925,7 +3927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E22" t="s">
         <v>68</v>
       </c>
@@ -3945,7 +3947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
         <v>72</v>
       </c>
@@ -3965,7 +3967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E24" t="s">
         <v>76</v>
       </c>
@@ -3985,7 +3987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E25" t="s">
         <v>80</v>
       </c>
@@ -4005,7 +4007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E26" t="s">
         <v>84</v>
       </c>
@@ -4025,7 +4027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E27" t="s">
         <v>88</v>
       </c>
@@ -4045,7 +4047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="28" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
         <v>92</v>
       </c>
@@ -4065,7 +4067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
         <v>96</v>
       </c>
@@ -4085,7 +4087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E30" t="s">
         <v>100</v>
       </c>
@@ -4105,7 +4107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E31" t="s">
         <v>104</v>
       </c>
@@ -4125,7 +4127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
         <v>108</v>
       </c>
@@ -4145,7 +4147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="33" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E33" t="s">
         <v>112</v>
       </c>
@@ -4165,7 +4167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="34" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E34" t="s">
         <v>116</v>
       </c>
@@ -4185,7 +4187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="35" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E35" t="s">
         <v>120</v>
       </c>
@@ -4205,7 +4207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="36" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E36" t="s">
         <v>389</v>
       </c>
@@ -4222,7 +4224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="37" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E37" t="s">
         <v>126</v>
       </c>
@@ -4242,7 +4244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="38" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E38" t="s">
         <v>130</v>
       </c>
@@ -4262,7 +4264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="39" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E39" t="s">
         <v>134</v>
       </c>
@@ -4282,7 +4284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="40" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E40" t="s">
         <v>137</v>
       </c>
@@ -4302,7 +4304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E41" t="s">
         <v>141</v>
       </c>
@@ -4322,7 +4324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E42" t="s">
         <v>145</v>
       </c>
@@ -4342,7 +4344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E43" t="s">
         <v>149</v>
       </c>
@@ -4362,7 +4364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E44" t="s">
         <v>153</v>
       </c>
@@ -4382,7 +4384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E45" t="s">
         <v>156</v>
       </c>
@@ -4402,7 +4404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E46" t="s">
         <v>134</v>
       </c>
@@ -4422,7 +4424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
         <v>163</v>
       </c>
@@ -4442,7 +4444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E48" t="s">
         <v>167</v>
       </c>
@@ -4462,7 +4464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E49" t="s">
         <v>171</v>
       </c>
@@ -4482,7 +4484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E50" t="s">
         <v>175</v>
       </c>
@@ -4502,7 +4504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E51" t="s">
         <v>179</v>
       </c>
@@ -4522,7 +4524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E52" t="s">
         <v>182</v>
       </c>
@@ -4542,7 +4544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E53" t="s">
         <v>186</v>
       </c>
@@ -4562,7 +4564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E54" t="s">
         <v>190</v>
       </c>
@@ -4582,7 +4584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E55" t="s">
         <v>194</v>
       </c>
@@ -4602,7 +4604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E56" t="s">
         <v>198</v>
       </c>
@@ -4622,7 +4624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E57" t="s">
         <v>202</v>
       </c>
@@ -4642,7 +4644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E58" t="s">
         <v>206</v>
       </c>
@@ -4662,7 +4664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E59" t="s">
         <v>210</v>
       </c>
@@ -4682,7 +4684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E60" t="s">
         <v>214</v>
       </c>
@@ -4702,7 +4704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="61" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E61" t="s">
         <v>218</v>
       </c>
@@ -4722,7 +4724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="62" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E62" t="s">
         <v>222</v>
       </c>
@@ -4742,7 +4744,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E63" t="s">
         <v>225</v>
       </c>
@@ -4762,7 +4764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="64" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E64" t="s">
         <v>229</v>
       </c>
@@ -4782,7 +4784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E65" t="s">
         <v>233</v>
       </c>
@@ -4802,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="66" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E66" t="s">
         <v>237</v>
       </c>
@@ -4822,7 +4824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="67" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E67" t="s">
         <v>240</v>
       </c>
@@ -4842,7 +4844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="68" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E68" t="s">
         <v>244</v>
       </c>
@@ -4862,7 +4864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="69" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E69" t="s">
         <v>248</v>
       </c>
@@ -4882,7 +4884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="70" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E70" t="s">
         <v>252</v>
       </c>
@@ -4902,7 +4904,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="71" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E71" t="s">
         <v>255</v>
       </c>
@@ -4922,7 +4924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="72" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E72" t="s">
         <v>259</v>
       </c>
@@ -4942,7 +4944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="73" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E73" t="s">
         <v>263</v>
       </c>
@@ -4962,7 +4964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="74" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E74" t="s">
         <v>266</v>
       </c>
@@ -4982,7 +4984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="75" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E75" t="s">
         <v>270</v>
       </c>
@@ -5002,7 +5004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="76" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E76" t="s">
         <v>40</v>
       </c>
@@ -5022,7 +5024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="77" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E77" t="s">
         <v>276</v>
       </c>
@@ -5042,7 +5044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="78" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E78" t="s">
         <v>280</v>
       </c>
@@ -5062,7 +5064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="79" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E79" t="s">
         <v>284</v>
       </c>
@@ -5082,7 +5084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="80" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E80" t="s">
         <v>287</v>
       </c>
@@ -5102,7 +5104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="81" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E81" t="s">
         <v>291</v>
       </c>
@@ -5122,7 +5124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="82" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E82" t="s">
         <v>295</v>
       </c>
@@ -5142,7 +5144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="83" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E83" t="s">
         <v>298</v>
       </c>
@@ -5162,7 +5164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="84" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E84" t="s">
         <v>302</v>
       </c>
@@ -5182,7 +5184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="85" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E85" t="s">
         <v>306</v>
       </c>
@@ -5202,7 +5204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="86" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E86" t="s">
         <v>310</v>
       </c>
@@ -5222,7 +5224,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="87" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E87" t="s">
         <v>313</v>
       </c>
@@ -5242,7 +5244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="88" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E88" t="s">
         <v>317</v>
       </c>
@@ -5262,7 +5264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="89" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E89" t="s">
         <v>321</v>
       </c>
@@ -5282,7 +5284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="90" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E90" t="s">
         <v>325</v>
       </c>
@@ -5302,7 +5304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="91" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E91" t="s">
         <v>329</v>
       </c>
@@ -5322,7 +5324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="92" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E92" t="s">
         <v>333</v>
       </c>
@@ -5342,7 +5344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="93" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E93" t="s">
         <v>337</v>
       </c>
@@ -5362,7 +5364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="94" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E94" t="s">
         <v>341</v>
       </c>
@@ -5382,7 +5384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="95" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E95" t="s">
         <v>344</v>
       </c>
@@ -5402,7 +5404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="96" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E96" t="s">
         <v>347</v>
       </c>
@@ -5422,7 +5424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="97" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E97" t="s">
         <v>351</v>
       </c>
@@ -5442,7 +5444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="98" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E98" t="s">
         <v>354</v>
       </c>
@@ -5462,7 +5464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="99" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E99" t="s">
         <v>358</v>
       </c>
@@ -5482,7 +5484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="100" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E100" t="s">
         <v>362</v>
       </c>
@@ -5502,7 +5504,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="101" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E101" t="s">
         <v>366</v>
       </c>
@@ -5522,7 +5524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="102" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E102" t="s">
         <v>370</v>
       </c>
@@ -5542,7 +5544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="103" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E103" t="s">
         <v>374</v>
       </c>
@@ -5562,7 +5564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="104" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E104" t="s">
         <v>378</v>
       </c>
@@ -5582,7 +5584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="5:10" x14ac:dyDescent="0.45">
+    <row r="105" spans="5:10" x14ac:dyDescent="0.2">
       <c r="E105" t="s">
         <v>382</v>
       </c>
@@ -5612,22 +5614,22 @@
   <dimension ref="D3:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="9.1328125" style="2"/>
-    <col min="5" max="5" width="9.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="9.1640625" style="2"/>
+    <col min="5" max="5" width="9.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="39" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.73046875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.59765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1328125" style="2"/>
+    <col min="7" max="7" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D3" s="2" t="s">
         <v>390</v>
       </c>
@@ -5650,7 +5652,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="4" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="4:10" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>4</v>
       </c>
@@ -5670,7 +5672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="4:10" x14ac:dyDescent="0.2">
       <c r="E5" t="s">
         <v>8</v>
       </c>
@@ -5684,13 +5686,13 @@
         <v>11</v>
       </c>
       <c r="I5">
-        <v>17</v>
+        <v>432178937489174</v>
       </c>
       <c r="J5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="4:10" x14ac:dyDescent="0.2">
       <c r="E6" t="s">
         <v>387</v>
       </c>
@@ -5710,7 +5712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="4:10" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>16</v>
       </c>
@@ -5730,7 +5732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="4:10" x14ac:dyDescent="0.2">
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8"/>
@@ -5738,7 +5740,7 @@
       <c r="I8"/>
       <c r="J8"/>
     </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="4:10" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>388</v>
       </c>
@@ -5758,7 +5760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="4:10" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>28</v>
       </c>

</xml_diff>